<commit_message>
actualizar lec 4 de busqueda
</commit_message>
<xml_diff>
--- a/Lecc4Find/FuncionesBusque.xlsx
+++ b/Lecc4Find/FuncionesBusque.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ReposGit\Excel_InicialDatos\Lecc4Find\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A078B6-3CB4-4EF5-A779-19F655AB2982}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663BF1DB-E8F7-4ED8-A60C-505FAA733495}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9ABDD8A0-D50D-4CBA-88BC-C6206BB5B64C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{9ABDD8A0-D50D-4CBA-88BC-C6206BB5B64C}"/>
   </bookViews>
   <sheets>
     <sheet name="1.CondicionesBuscar" sheetId="2" r:id="rId1"/>
@@ -18,10 +18,13 @@
     <sheet name="03.IndiceCoincir" sheetId="9" r:id="rId3"/>
     <sheet name="04.buscarx" sheetId="6" r:id="rId4"/>
     <sheet name="05.DESAFIO1" sheetId="7" r:id="rId5"/>
+    <sheet name="05.DESAFIO2" sheetId="10" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'03.IndiceCoincir'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'04.buscarx'!#REF!</definedName>
+    <definedName name="Table1">'05.DESAFIO1'!$J$12:$K$20</definedName>
+    <definedName name="Table2">'05.DESAFIO1'!$M$12:$N$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,8 +43,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="190">
   <si>
     <t>FUNCION</t>
   </si>
@@ -265,9 +290,6 @@
     <t>QUE QUIERO TRAER?</t>
   </si>
   <si>
-    <t>=COINDIDIR()</t>
-  </si>
-  <si>
     <t>COMO LO ENCUENTRO?</t>
   </si>
   <si>
@@ -278,6 +300,342 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>=COINCIDIR()</t>
+  </si>
+  <si>
+    <t>MIENTRAS MENOS CLICS NECESITAS PARA HACER LA BUSQUEDA ES MEJOR</t>
+  </si>
+  <si>
+    <t>Henderson</t>
+  </si>
+  <si>
+    <t>Mazden</t>
+  </si>
+  <si>
+    <t>Albertson</t>
+  </si>
+  <si>
+    <t>Perez</t>
+  </si>
+  <si>
+    <t>Mendez</t>
+  </si>
+  <si>
+    <t>Gonzolez</t>
+  </si>
+  <si>
+    <t>Deerberg</t>
+  </si>
+  <si>
+    <t>Gomez</t>
+  </si>
+  <si>
+    <t>Talisman</t>
+  </si>
+  <si>
+    <t>Hardy</t>
+  </si>
+  <si>
+    <t>Klorber</t>
+  </si>
+  <si>
+    <t>Darvin</t>
+  </si>
+  <si>
+    <t>King</t>
+  </si>
+  <si>
+    <t>Nester</t>
+  </si>
+  <si>
+    <t>Jackson</t>
+  </si>
+  <si>
+    <t>Bateos</t>
+  </si>
+  <si>
+    <t>Promedio Bateo</t>
+  </si>
+  <si>
+    <t>Jugador</t>
+  </si>
+  <si>
+    <t>Jugador Buscado</t>
+  </si>
+  <si>
+    <t>PromedioBateo</t>
+  </si>
+  <si>
+    <t>Commission</t>
+  </si>
+  <si>
+    <t>Benson</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Davidson</t>
+  </si>
+  <si>
+    <t>Ellison</t>
+  </si>
+  <si>
+    <t>Hernandez</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Oswald</t>
+  </si>
+  <si>
+    <t>Reginald</t>
+  </si>
+  <si>
+    <t>Veras</t>
+  </si>
+  <si>
+    <t>Wilmington</t>
+  </si>
+  <si>
+    <t>FORMA 1</t>
+  </si>
+  <si>
+    <t>Repre.Venta</t>
+  </si>
+  <si>
+    <t>Anios</t>
+  </si>
+  <si>
+    <t>Ventas</t>
+  </si>
+  <si>
+    <t>Ratio Venta</t>
+  </si>
+  <si>
+    <t>&lt;3 anios trabajo</t>
+  </si>
+  <si>
+    <t>3+ anios trabajo</t>
+  </si>
+  <si>
+    <t>Escala Venta</t>
+  </si>
+  <si>
+    <t>FORMA 2</t>
+  </si>
+  <si>
+    <t>USO DE RANGOS CON NOMBRE Y ANIOS DE TRABAJO</t>
+  </si>
+  <si>
+    <t>USANDO SI.ERROR EN CASO QUE LA BUSQUEDA DEVUELVA ERROR</t>
+  </si>
+  <si>
+    <t>VALORES MENORES</t>
+  </si>
+  <si>
+    <t>FORMA 3</t>
+  </si>
+  <si>
+    <t>USANDO INDICE Y COINCIDIR</t>
+  </si>
+  <si>
+    <t>DECIDIR BUSCAR EN UNA TABLA O EN LA OTRA CON RANGOS NOMBRADOS</t>
+  </si>
+  <si>
+    <t>Widgets</t>
+  </si>
+  <si>
+    <t>Sprockets</t>
+  </si>
+  <si>
+    <t>Snapholytes</t>
+  </si>
+  <si>
+    <t>Combined</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>QUE TE PERMITA ARRASTRAR DE MANERA TANTO HORIZONTAL COMO VERTICAL</t>
+  </si>
+  <si>
+    <t>1. REALIZA LA BUSQUEDA DE LOS DATOS SOLICITADOS EN LA TABLA 'B' USANDO UNA SOLA FORMULA</t>
+  </si>
+  <si>
+    <t>Make:</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>Make</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Model:</t>
+  </si>
+  <si>
+    <t>Sequoia</t>
+  </si>
+  <si>
+    <t>Chevy</t>
+  </si>
+  <si>
+    <t>Suburban</t>
+  </si>
+  <si>
+    <t>C-094</t>
+  </si>
+  <si>
+    <t>Code:</t>
+  </si>
+  <si>
+    <t>T-871</t>
+  </si>
+  <si>
+    <t>Tahoe</t>
+  </si>
+  <si>
+    <t>C-823</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>Explorer</t>
+  </si>
+  <si>
+    <t>F-772</t>
+  </si>
+  <si>
+    <t>Escape</t>
+  </si>
+  <si>
+    <t>F-229</t>
+  </si>
+  <si>
+    <t>Honda</t>
+  </si>
+  <si>
+    <t>Pilot</t>
+  </si>
+  <si>
+    <t>I-897</t>
+  </si>
+  <si>
+    <t>CR-V</t>
+  </si>
+  <si>
+    <t>I-900</t>
+  </si>
+  <si>
+    <t>Jeep</t>
+  </si>
+  <si>
+    <t>Compass</t>
+  </si>
+  <si>
+    <t>J-983</t>
+  </si>
+  <si>
+    <t>Grand Cherokee</t>
+  </si>
+  <si>
+    <t>J-701</t>
+  </si>
+  <si>
+    <t>Nissan</t>
+  </si>
+  <si>
+    <t>N-231</t>
+  </si>
+  <si>
+    <t>Land Cruiser</t>
+  </si>
+  <si>
+    <t>T-981</t>
+  </si>
+  <si>
+    <t>2. ENCUENTRA EL CODIGO DEL AUTOMOVIL EN BASE A  LOS CRITERIOS DE 'MAKE' Y 'MODEL'</t>
+  </si>
+  <si>
+    <t>COINCIDIR FILAS Y COLUMNAS NO HACE FALTA USAR BUSCARH</t>
+  </si>
+  <si>
+    <t>VALOR 2A</t>
+  </si>
+  <si>
+    <t>VALOR 3</t>
+  </si>
+  <si>
+    <t>CODIGOS</t>
+  </si>
+  <si>
+    <t>ASD</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>DFS</t>
+  </si>
+  <si>
+    <t>FGD</t>
+  </si>
+  <si>
+    <t>EFEW</t>
+  </si>
+  <si>
+    <t>ERET</t>
   </si>
 </sst>
 </file>
@@ -288,7 +646,7 @@
     <numFmt numFmtId="44" formatCode="_ &quot;$&quot;* #,##0.00_ ;_ &quot;$&quot;* \-#,##0.00_ ;_ &quot;$&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,16 +691,73 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="63"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="63"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="62"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -365,13 +780,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -394,11 +834,67 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -509,8 +1005,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="212716" y="182946"/>
-          <a:ext cx="3399163" cy="585619"/>
+          <a:off x="208906" y="184851"/>
+          <a:ext cx="3397258" cy="589429"/>
           <a:chOff x="2791304" y="276225"/>
           <a:chExt cx="4697162" cy="879193"/>
         </a:xfrm>
@@ -2506,8 +3002,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="212716" y="182946"/>
-          <a:ext cx="3042929" cy="595144"/>
+          <a:off x="208906" y="184851"/>
+          <a:ext cx="3050549" cy="604669"/>
           <a:chOff x="2791304" y="276225"/>
           <a:chExt cx="4697162" cy="879193"/>
         </a:xfrm>
@@ -3198,8 +3694,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="212716" y="182946"/>
-          <a:ext cx="2501909" cy="585619"/>
+          <a:off x="208906" y="184851"/>
+          <a:ext cx="2511434" cy="589429"/>
           <a:chOff x="2791304" y="276225"/>
           <a:chExt cx="6104916" cy="879193"/>
         </a:xfrm>
@@ -3658,7 +4154,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
+      <xdr:colOff>15240</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>36450</xdr:rowOff>
     </xdr:to>
@@ -3933,13 +4429,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>478155</xdr:colOff>
+      <xdr:colOff>668655</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>264795</xdr:colOff>
+      <xdr:colOff>59055</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
     </xdr:to>
@@ -3970,7 +4466,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6078855" y="0"/>
+          <a:off x="6276975" y="0"/>
           <a:ext cx="1813560" cy="510540"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3983,15 +4479,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>862965</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>71829</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1092909</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>70485</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4020,7 +4516,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6257925" y="537210"/>
+          <a:off x="6471285" y="598170"/>
           <a:ext cx="1441524" cy="569595"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4189,25 +4685,311 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>249060</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>370980</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>36450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectángulo 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{066246CE-0D13-4206-AE9A-184E01DD56C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="8046720" cy="1133730"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00203C"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00203C"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>208906</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1971</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>42760</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="3" name="Grupo 2" descr="&quot;&quot;" title="Lista de comprobación de elementos de vacaciones">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E00ECEE-020A-4863-A460-F040196B82AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="208906" y="184851"/>
+          <a:ext cx="2511434" cy="589429"/>
+          <a:chOff x="2791304" y="276225"/>
+          <a:chExt cx="6104916" cy="879193"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="4" name="Lista de comprobación de elementos de vacaciones" descr="&quot;&quot;" title="Lista de comprobación de elementos de vacaciones">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2597D706-C643-4B98-8B52-90D63F4DC9D0}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="2799789" y="276225"/>
+            <a:ext cx="6096431" cy="879193"/>
+            <a:chOff x="3686175" y="152400"/>
+            <a:chExt cx="3872816" cy="879193"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="Cuadro de texto 321">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3328778E-D62E-4FCF-AA64-373328724E82}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3686175" y="152400"/>
+              <a:ext cx="2667000" cy="571500"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0"/>
+              <a:r>
+                <a:rPr lang="es" sz="2000" b="1" spc="50" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mj-lt"/>
+                </a:rPr>
+                <a:t>LECCION 4</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0"/>
+              <a:endParaRPr lang="en-US" sz="2000" b="1" spc="50" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="Cuadro de texto 322">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E143BD0-FACA-4DC9-8FC7-ECD1E404931D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3695192" y="704689"/>
+              <a:ext cx="3863799" cy="326904"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" spc="200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>DESAFIO 2</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="5" name="Conector recto 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB183CEB-EC25-4DCD-A239-917C0A9A24BC}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2791304" y="768343"/>
+            <a:ext cx="4383015" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>516255</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>744855</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Gráfico 17" descr="Lluvia de ideas con relleno sólido">
+        <xdr:cNvPr id="8" name="Imagen 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{970E0362-8710-4AEB-9ED0-D01C5FF8651E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6236343-D825-4FD1-8DFD-4A065B083052}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4216,13 +4998,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId10"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -4232,8 +5011,217 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12189600" y="5331600"/>
-          <a:ext cx="914400" cy="914400"/>
+          <a:off x="6063615" y="0"/>
+          <a:ext cx="1813560" cy="510540"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>710565</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>567129</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>62865</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68A79E25-6488-4A29-B836-07128939FAB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6257925" y="590550"/>
+          <a:ext cx="1441524" cy="569595"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Gráfico 9" descr="Publicidad">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EDB2CF4-6A36-4AF6-8528-F60684008F0C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2316480" y="0"/>
+          <a:ext cx="944880" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>731025</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>92850</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Gráfico 10" descr="Inteligencia artificial">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6454CC8A-E4E5-4A83-81EC-917FCF72D57F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId6"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3108465" y="0"/>
+          <a:ext cx="946785" cy="883920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>776250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>157125</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Gráfico 11" descr="Pared de ladrillo de edificio">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{005CFDC1-3968-4B62-BE9C-2FD2371CA298}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId8"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3946170" y="0"/>
+          <a:ext cx="965835" cy="876300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4547,8 +5535,8 @@
   </sheetPr>
   <dimension ref="B9:N65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4569,7 +5557,7 @@
         <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="21" x14ac:dyDescent="0.4">
@@ -5462,11 +6450,11 @@
         <v>15</v>
       </c>
       <c r="E65" s="8" t="str">
-        <f t="shared" ref="E61:E65" si="9">VLOOKUP(B65,$L$59:$M$63,2,0)</f>
+        <f t="shared" ref="E65" si="9">VLOOKUP(B65,$L$59:$M$63,2,0)</f>
         <v>NORTE</v>
       </c>
       <c r="F65" t="e">
-        <f t="shared" ref="F61:F65" si="10">VLOOKUP(B65,$L$59:$M$63,2,1)</f>
+        <f t="shared" ref="F65" si="10">VLOOKUP(B65,$L$59:$M$63,2,1)</f>
         <v>#N/A</v>
       </c>
       <c r="G65" t="str">
@@ -5491,8 +6479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40B2E87-9AA1-4B2A-8E5A-DDF3639D35E8}">
   <dimension ref="A16:X46"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView showGridLines="0" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6007,10 +6995,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9947BE7E-66F1-44B5-81C4-58BF1FADF6ED}">
-  <dimension ref="A9:M53"/>
+  <dimension ref="A9:M97"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6310,10 +7298,10 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B44" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" t="s">
         <v>74</v>
-      </c>
-      <c r="C44" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
@@ -6477,7 +7465,7 @@
         <v>4</v>
       </c>
       <c r="C52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D52">
         <f t="shared" si="4"/>
@@ -6494,7 +7482,7 @@
         <v>62487</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M52" s="4">
         <v>22196</v>
@@ -6508,7 +7496,7 @@
         <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D53">
         <f t="shared" si="4"/>
@@ -6525,24 +7513,463 @@
         <v>43254</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M53" s="4">
         <v>22196</v>
       </c>
     </row>
+    <row r="57" spans="1:13" ht="21" x14ac:dyDescent="0.4">
+      <c r="C57" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B59" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D59" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="F59" t="s">
+        <v>98</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B61">
+        <v>9</v>
+      </c>
+      <c r="C61">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="D61" t="s">
+        <v>81</v>
+      </c>
+      <c r="F61" t="s">
+        <v>99</v>
+      </c>
+      <c r="H61" s="4" t="str">
+        <f>VLOOKUP($H$59,$B$59:$D$74,2)</f>
+        <v>Promedio Bateo</v>
+      </c>
+      <c r="J61" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(H61)</f>
+        <v>=BUSCARV($H$59;$B$59:$D$74;2)</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B62">
+        <v>12</v>
+      </c>
+      <c r="C62">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="D62" t="s">
+        <v>82</v>
+      </c>
+      <c r="F62" t="s">
+        <v>95</v>
+      </c>
+      <c r="H62" s="4" t="str">
+        <f>VLOOKUP($H$59,$B$59:$D$74,1)</f>
+        <v>Bateos</v>
+      </c>
+      <c r="J62" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(H62)</f>
+        <v>=BUSCARV($H$59;$B$59:$D$74;1)</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B63">
+        <v>14</v>
+      </c>
+      <c r="C63">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="D63" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B64">
+        <v>16</v>
+      </c>
+      <c r="C64">
+        <v>0.313</v>
+      </c>
+      <c r="D64" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B65">
+        <v>23</v>
+      </c>
+      <c r="C65">
+        <v>0.217</v>
+      </c>
+      <c r="D65" t="s">
+        <v>85</v>
+      </c>
+      <c r="F65" t="s">
+        <v>96</v>
+      </c>
+      <c r="H65" s="4">
+        <f>INDEX($C$60:$C$74,MATCH($H$59,$D$60:$D$74,0))</f>
+        <v>0.3</v>
+      </c>
+      <c r="J65" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(H65)</f>
+        <v>=INDICE($C$60:$C$74;COINCIDIR($H$59;$D$60:$D$74;0))</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B66">
+        <v>24</v>
+      </c>
+      <c r="C66">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="D66" t="s">
+        <v>86</v>
+      </c>
+      <c r="F66" t="s">
+        <v>95</v>
+      </c>
+      <c r="H66" s="4">
+        <f>INDEX($B$60:$B$74,MATCH($H$59,$D$60:$D$74,0))</f>
+        <v>30</v>
+      </c>
+      <c r="J66" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(H66)</f>
+        <v>=INDICE($B$60:$B$74;COINCIDIR($H$59;$D$60:$D$74;0))</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <v>25</v>
+      </c>
+      <c r="C67">
+        <v>0.16</v>
+      </c>
+      <c r="D67" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B68">
+        <v>28</v>
+      </c>
+      <c r="C68">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="D68" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>30</v>
+      </c>
+      <c r="C69">
+        <v>0.3</v>
+      </c>
+      <c r="D69" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B70">
+        <v>36</v>
+      </c>
+      <c r="C70">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="D70" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B71">
+        <v>41</v>
+      </c>
+      <c r="C71">
+        <v>0.39</v>
+      </c>
+      <c r="D71" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B72">
+        <v>43</v>
+      </c>
+      <c r="C72">
+        <v>0.186</v>
+      </c>
+      <c r="D72" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B73">
+        <v>44</v>
+      </c>
+      <c r="C73">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="D73" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B74">
+        <v>51</v>
+      </c>
+      <c r="C74">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="D74" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="A78" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B80" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="J80" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B81" cm="1">
+        <f t="array" ref="B81">INDEX($H$81:$J$81,,MATCH(B$80,$H$80:$J$80,0))</f>
+        <v>1234</v>
+      </c>
+      <c r="C81" cm="1">
+        <f t="array" ref="C81">INDEX($H$81:$J$81,,MATCH(C$80,$H$80:$J$80,0))</f>
+        <v>456</v>
+      </c>
+      <c r="D81" cm="1">
+        <f t="array" ref="D81">INDEX($H$81:$J$81,,MATCH(D$80,$H$80:$J$80,0))</f>
+        <v>567</v>
+      </c>
+      <c r="H81">
+        <v>1234</v>
+      </c>
+      <c r="I81">
+        <v>456</v>
+      </c>
+      <c r="J81">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B82" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B81)</f>
+        <v>=INDICE($H$81:$J$81;;COINCIDIR(B$80;$H$80:$J$80;0))</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" ref="C82:D82" ca="1" si="6">_xlfn.FORMULATEXT(C81)</f>
+        <v>=INDICE($H$81:$J$81;;COINCIDIR(C$80;$H$80:$J$80;0))</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>=INDICE($H$81:$J$81;;COINCIDIR(D$80;$H$80:$J$80;0))</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="K93" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>123</v>
+      </c>
+      <c r="B94" t="str">
+        <f>INDEX($I$94:$K$97,MATCH($A94,$H$94:$H$97,0),MATCH(B$93,$I$93:$K$93,0))</f>
+        <v>ASD</v>
+      </c>
+      <c r="C94">
+        <f t="shared" ref="C94:D97" si="7">INDEX($I$94:$K$97,MATCH($A94,$H$94:$H$97,0),MATCH(C$93,$I$93:$K$93,0))</f>
+        <v>324</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="7"/>
+        <v>56</v>
+      </c>
+      <c r="H94">
+        <v>123</v>
+      </c>
+      <c r="I94" t="s">
+        <v>184</v>
+      </c>
+      <c r="J94">
+        <v>324</v>
+      </c>
+      <c r="K94">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>1234</v>
+      </c>
+      <c r="B95" t="str">
+        <f t="shared" ref="B95:B97" si="8">INDEX($I$94:$K$97,MATCH($A95,$H$94:$H$97,0),MATCH(B$93,$I$93:$K$93,0))</f>
+        <v>DS</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="7"/>
+        <v>344</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="7"/>
+        <v>765</v>
+      </c>
+      <c r="H95">
+        <v>1234</v>
+      </c>
+      <c r="I95" t="s">
+        <v>185</v>
+      </c>
+      <c r="J95">
+        <v>344</v>
+      </c>
+      <c r="K95">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>12345</v>
+      </c>
+      <c r="B96" t="str">
+        <f t="shared" si="8"/>
+        <v>DFS</v>
+      </c>
+      <c r="C96" t="str">
+        <f t="shared" si="7"/>
+        <v>EFEW</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="7"/>
+        <v>453</v>
+      </c>
+      <c r="H96">
+        <v>12345</v>
+      </c>
+      <c r="I96" t="s">
+        <v>186</v>
+      </c>
+      <c r="J96" t="s">
+        <v>188</v>
+      </c>
+      <c r="K96">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>123445</v>
+      </c>
+      <c r="B97" t="str">
+        <f t="shared" si="8"/>
+        <v>FGD</v>
+      </c>
+      <c r="C97" t="str">
+        <f t="shared" si="7"/>
+        <v>ERET</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="7"/>
+        <v>23</v>
+      </c>
+      <c r="H97">
+        <v>123445</v>
+      </c>
+      <c r="I97" t="s">
+        <v>187</v>
+      </c>
+      <c r="J97" t="s">
+        <v>189</v>
+      </c>
+      <c r="K97">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A66D965B-CD9F-4069-906C-76269E752F0A}">
-  <dimension ref="A1"/>
+  <dimension ref="B10:J25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6555,7 +7982,212 @@
     <col min="7" max="10" width="7.88671875" customWidth="1"/>
     <col min="11" max="12" width="10" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="D12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" t="s">
+        <v>96</v>
+      </c>
+      <c r="H12" s="4">
+        <f>_xlfn.XLOOKUP($H$10,$D$11:$D$25,$C$11:$C$25,,0)</f>
+        <v>0.3</v>
+      </c>
+      <c r="J12" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(H12)</f>
+        <v>=BUSCARX($H$10;$D$11:$D$25;$C$11:$C$25;;0)</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="D13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" s="4">
+        <f>_xlfn.XLOOKUP($H$10,$D$11:$D$25,$B$11:$B$25,,0)</f>
+        <v>30</v>
+      </c>
+      <c r="J13" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(H13)</f>
+        <v>=BUSCARX($H$10;$D$11:$D$25;$B$11:$B$25;;0)</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="D14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>0.313</v>
+      </c>
+      <c r="D15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>0.217</v>
+      </c>
+      <c r="D16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>24</v>
+      </c>
+      <c r="C17">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="D17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <v>0.16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>28</v>
+      </c>
+      <c r="C19">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="D19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>30</v>
+      </c>
+      <c r="C20">
+        <v>0.3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>36</v>
+      </c>
+      <c r="C21">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="D21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>41</v>
+      </c>
+      <c r="C22">
+        <v>0.39</v>
+      </c>
+      <c r="D22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>43</v>
+      </c>
+      <c r="C23">
+        <v>0.186</v>
+      </c>
+      <c r="D23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>44</v>
+      </c>
+      <c r="C24">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="D24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>51</v>
+      </c>
+      <c r="C25">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="D25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -6564,10 +8196,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97223706-25BC-4B5C-AFEB-83702A354A86}">
-  <dimension ref="A1"/>
+  <dimension ref="A9:N59"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView showGridLines="0" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6575,13 +8207,1624 @@
     <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="5" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="9" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="I12" s="20"/>
+      <c r="J12" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="K12" s="22"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="N12" s="22"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" s="25">
+        <v>2</v>
+      </c>
+      <c r="C13" s="26">
+        <v>120000</v>
+      </c>
+      <c r="D13" s="27">
+        <f>VLOOKUP(C13,IF(B13&lt;3,Table1,Table2),2)</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E13" s="26">
+        <f>C13*D13</f>
+        <v>8400</v>
+      </c>
+      <c r="F13" s="41" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(D13)</f>
+        <v>=BUSCARV(C13;SI(B13&lt;3;Table1;Table2);2)</v>
+      </c>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="K13" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="L13" s="20"/>
+      <c r="M13" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="N13" s="28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="30">
+        <v>1</v>
+      </c>
+      <c r="C14" s="31">
+        <v>210921</v>
+      </c>
+      <c r="D14" s="32">
+        <f t="shared" ref="D14:D23" si="0">VLOOKUP(C14,IF(B14&lt;3,Table1,Table2),2)</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E14" s="31">
+        <f t="shared" ref="E14:E23" si="1">C14*D14</f>
+        <v>14764.470000000001</v>
+      </c>
+      <c r="F14" s="41" t="str">
+        <f t="shared" ref="F14:F23" ca="1" si="2">_xlfn.FORMULATEXT(D14)</f>
+        <v>=BUSCARV(C14;SI(B14&lt;3;Table1;Table2);2)</v>
+      </c>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="J14" s="33">
+        <v>0</v>
+      </c>
+      <c r="K14" s="34">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M14" s="33">
+        <v>0</v>
+      </c>
+      <c r="N14" s="34">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="30">
+        <v>1</v>
+      </c>
+      <c r="C15" s="31">
+        <v>100000</v>
+      </c>
+      <c r="D15" s="32">
+        <f t="shared" si="0"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E15" s="31">
+        <f t="shared" si="1"/>
+        <v>7000.0000000000009</v>
+      </c>
+      <c r="F15" s="41" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>=BUSCARV(C15;SI(B15&lt;3;Table1;Table2);2)</v>
+      </c>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="J15" s="33">
+        <f>J14+5000</f>
+        <v>5000</v>
+      </c>
+      <c r="K15" s="34">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="M15" s="33">
+        <v>50000</v>
+      </c>
+      <c r="N15" s="34">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="30">
+        <v>2</v>
+      </c>
+      <c r="C16" s="31">
+        <v>87401</v>
+      </c>
+      <c r="D16" s="32">
+        <f t="shared" si="0"/>
+        <v>0.06</v>
+      </c>
+      <c r="E16" s="31">
+        <f t="shared" si="1"/>
+        <v>5244.0599999999995</v>
+      </c>
+      <c r="F16" s="41" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>=BUSCARV(C16;SI(B16&lt;3;Table1;Table2);2)</v>
+      </c>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="J16" s="33">
+        <f>J15+5000</f>
+        <v>10000</v>
+      </c>
+      <c r="K16" s="34">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="M16" s="33">
+        <v>100000</v>
+      </c>
+      <c r="N16" s="34">
+        <v>7.2499999999999995E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="30">
+        <v>6</v>
+      </c>
+      <c r="C17" s="31">
+        <v>310983</v>
+      </c>
+      <c r="D17" s="32">
+        <f t="shared" si="0"/>
+        <v>9.2499999999999999E-2</v>
+      </c>
+      <c r="E17" s="31">
+        <f t="shared" si="1"/>
+        <v>28765.927499999998</v>
+      </c>
+      <c r="F17" s="41" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>=BUSCARV(C17;SI(B17&lt;3;Table1;Table2);2)</v>
+      </c>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="J17" s="33">
+        <v>20000</v>
+      </c>
+      <c r="K17" s="34">
+        <v>0.05</v>
+      </c>
+      <c r="M17" s="33">
+        <v>200000</v>
+      </c>
+      <c r="N17" s="34">
+        <v>8.2500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" s="30">
+        <v>3</v>
+      </c>
+      <c r="C18" s="31">
+        <v>43902</v>
+      </c>
+      <c r="D18" s="32">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="E18" s="31">
+        <f t="shared" si="1"/>
+        <v>878.04</v>
+      </c>
+      <c r="F18" s="41" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>=BUSCARV(C18;SI(B18&lt;3;Table1;Table2);2)</v>
+      </c>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="J18" s="33">
+        <v>50000</v>
+      </c>
+      <c r="K18" s="34">
+        <v>0.06</v>
+      </c>
+      <c r="M18" s="33">
+        <v>300000</v>
+      </c>
+      <c r="N18" s="34">
+        <v>9.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" s="30">
+        <v>2</v>
+      </c>
+      <c r="C19" s="31">
+        <v>121021</v>
+      </c>
+      <c r="D19" s="32">
+        <f t="shared" si="0"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E19" s="31">
+        <f t="shared" si="1"/>
+        <v>8471.4700000000012</v>
+      </c>
+      <c r="F19" s="41" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>=BUSCARV(C19;SI(B19&lt;3;Table1;Table2);2)</v>
+      </c>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="J19" s="33">
+        <v>100000</v>
+      </c>
+      <c r="K19" s="34">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M19" s="33">
+        <v>500000</v>
+      </c>
+      <c r="N19" s="34">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="30">
+        <v>3</v>
+      </c>
+      <c r="C20" s="31">
+        <v>908</v>
+      </c>
+      <c r="D20" s="32">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="E20" s="31">
+        <f t="shared" si="1"/>
+        <v>18.16</v>
+      </c>
+      <c r="F20" s="41" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>=BUSCARV(C20;SI(B20&lt;3;Table1;Table2);2)</v>
+      </c>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="J20" s="33">
+        <v>250000</v>
+      </c>
+      <c r="K20" s="34">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" s="30">
+        <v>1</v>
+      </c>
+      <c r="C21" s="31">
+        <v>0</v>
+      </c>
+      <c r="D21" s="32">
+        <f t="shared" si="0"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E21" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="41" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>=BUSCARV(C21;SI(B21&lt;3;Table1;Table2);2)</v>
+      </c>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="B22" s="30">
+        <v>4</v>
+      </c>
+      <c r="C22" s="31">
+        <v>359832</v>
+      </c>
+      <c r="D22" s="32">
+        <f t="shared" si="0"/>
+        <v>9.2499999999999999E-2</v>
+      </c>
+      <c r="E22" s="31">
+        <f t="shared" si="1"/>
+        <v>33284.46</v>
+      </c>
+      <c r="F22" s="41" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>=BUSCARV(C22;SI(B22&lt;3;Table1;Table2);2)</v>
+      </c>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" s="30">
+        <v>4</v>
+      </c>
+      <c r="C23" s="31">
+        <v>502983</v>
+      </c>
+      <c r="D23" s="32">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="E23" s="31">
+        <f t="shared" si="1"/>
+        <v>50298.3</v>
+      </c>
+      <c r="F23" s="41" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>=BUSCARV(C23;SI(B23&lt;3;Table1;Table2);2)</v>
+      </c>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="D30" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="E30" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="J30" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="K30" s="38"/>
+      <c r="M30" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="N30" s="37"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="4">
+        <v>2</v>
+      </c>
+      <c r="C31" s="40">
+        <v>120000</v>
+      </c>
+      <c r="D31" s="43">
+        <f>IFERROR(VLOOKUP(C31,J31:K38,2,1),VLOOKUP(C31,$M$31:$N$37,2,1))</f>
+        <v>0.08</v>
+      </c>
+      <c r="E31" s="4">
+        <f>C31*D31</f>
+        <v>9600</v>
+      </c>
+      <c r="F31" s="12" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(D31)</f>
+        <v>=SI.ERROR(BUSCARV(C31;J31:K38;2;1);BUSCARV(C31;$M$31:$N$37;2;1))</v>
+      </c>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="J31" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="K31" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="M31" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="N31" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" s="4">
+        <v>1</v>
+      </c>
+      <c r="C32" s="40">
+        <v>210921</v>
+      </c>
+      <c r="D32" s="43">
+        <f t="shared" ref="D32:D41" si="3">IFERROR(VLOOKUP(C32,J32:K39,2,1),VLOOKUP(C32,$M$31:$N$37,2,1))</f>
+        <v>0.08</v>
+      </c>
+      <c r="E32" s="4">
+        <f t="shared" ref="E32:E41" si="4">C32*D32</f>
+        <v>16873.68</v>
+      </c>
+      <c r="F32" s="12" t="str">
+        <f t="shared" ref="F32:F41" ca="1" si="5">_xlfn.FORMULATEXT(D32)</f>
+        <v>=SI.ERROR(BUSCARV(C32;J32:K39;2;1);BUSCARV(C32;$M$31:$N$37;2;1))</v>
+      </c>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="J32" s="40">
+        <v>0</v>
+      </c>
+      <c r="K32" s="39">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M32" s="40">
+        <v>0</v>
+      </c>
+      <c r="N32" s="39">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" s="4">
+        <v>1</v>
+      </c>
+      <c r="C33" s="40">
+        <v>100000</v>
+      </c>
+      <c r="D33" s="43">
+        <f t="shared" si="3"/>
+        <v>0.08</v>
+      </c>
+      <c r="E33" s="4">
+        <f t="shared" si="4"/>
+        <v>8000</v>
+      </c>
+      <c r="F33" s="12" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>=SI.ERROR(BUSCARV(C33;J33:K40;2;1);BUSCARV(C33;$M$31:$N$37;2;1))</v>
+      </c>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="J33" s="40">
+        <v>5000</v>
+      </c>
+      <c r="K33" s="39">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="M33" s="40">
+        <v>50000</v>
+      </c>
+      <c r="N33" s="39">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="4">
+        <v>2</v>
+      </c>
+      <c r="C34" s="40">
+        <v>87401</v>
+      </c>
+      <c r="D34" s="43">
+        <f t="shared" si="3"/>
+        <v>0.08</v>
+      </c>
+      <c r="E34" s="4">
+        <f t="shared" si="4"/>
+        <v>6992.08</v>
+      </c>
+      <c r="F34" s="12" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>=SI.ERROR(BUSCARV(C34;J34:K41;2;1);BUSCARV(C34;$M$31:$N$37;2;1))</v>
+      </c>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="J34" s="40">
+        <v>10000</v>
+      </c>
+      <c r="K34" s="39">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="M34" s="40">
+        <v>100000</v>
+      </c>
+      <c r="N34" s="39">
+        <v>7.2499999999999995E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" s="4">
+        <v>6</v>
+      </c>
+      <c r="C35" s="40">
+        <v>310983</v>
+      </c>
+      <c r="D35" s="43">
+        <f t="shared" si="3"/>
+        <v>0.08</v>
+      </c>
+      <c r="E35" s="4">
+        <f t="shared" si="4"/>
+        <v>24878.639999999999</v>
+      </c>
+      <c r="F35" s="12" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>=SI.ERROR(BUSCARV(C35;J35:K42;2;1);BUSCARV(C35;$M$31:$N$37;2;1))</v>
+      </c>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="J35" s="40">
+        <v>20000</v>
+      </c>
+      <c r="K35" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="M35" s="40">
+        <v>200000</v>
+      </c>
+      <c r="N35" s="39">
+        <v>8.2500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" s="4">
+        <v>3</v>
+      </c>
+      <c r="C36" s="40">
+        <v>43902</v>
+      </c>
+      <c r="D36" s="43">
+        <f t="shared" si="3"/>
+        <v>0.08</v>
+      </c>
+      <c r="E36" s="4">
+        <f t="shared" si="4"/>
+        <v>3512.16</v>
+      </c>
+      <c r="F36" s="12" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>=SI.ERROR(BUSCARV(C36;J36:K43;2;1);BUSCARV(C36;$M$31:$N$37;2;1))</v>
+      </c>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="J36" s="40">
+        <v>25000</v>
+      </c>
+      <c r="K36" s="39">
+        <v>0.06</v>
+      </c>
+      <c r="M36" s="40">
+        <v>300000</v>
+      </c>
+      <c r="N36" s="39">
+        <v>9.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37" s="4">
+        <v>2</v>
+      </c>
+      <c r="C37" s="40">
+        <v>121021</v>
+      </c>
+      <c r="D37" s="43">
+        <f t="shared" si="3"/>
+        <v>0.08</v>
+      </c>
+      <c r="E37" s="4">
+        <f t="shared" si="4"/>
+        <v>9681.68</v>
+      </c>
+      <c r="F37" s="12" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>=SI.ERROR(BUSCARV(C37;J37:K44;2;1);BUSCARV(C37;$M$31:$N$37;2;1))</v>
+      </c>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="J37" s="40">
+        <v>30000</v>
+      </c>
+      <c r="K37" s="39">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M37" s="40">
+        <v>500000</v>
+      </c>
+      <c r="N37" s="39">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="4">
+        <v>3</v>
+      </c>
+      <c r="C38" s="40">
+        <v>908</v>
+      </c>
+      <c r="D38" s="43">
+        <f t="shared" si="3"/>
+        <v>0.02</v>
+      </c>
+      <c r="E38" s="4">
+        <f t="shared" si="4"/>
+        <v>18.16</v>
+      </c>
+      <c r="F38" s="12" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>=SI.ERROR(BUSCARV(C38;J38:K45;2;1);BUSCARV(C38;$M$31:$N$37;2;1))</v>
+      </c>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="J38" s="40">
+        <v>35000</v>
+      </c>
+      <c r="K38" s="39">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="4">
+        <v>1</v>
+      </c>
+      <c r="C39" s="40">
+        <v>0</v>
+      </c>
+      <c r="D39" s="43">
+        <f t="shared" si="3"/>
+        <v>0.02</v>
+      </c>
+      <c r="E39" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="12" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>=SI.ERROR(BUSCARV(C39;J39:K46;2;1);BUSCARV(C39;$M$31:$N$37;2;1))</v>
+      </c>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" s="4">
+        <v>4</v>
+      </c>
+      <c r="C40" s="40">
+        <v>359832</v>
+      </c>
+      <c r="D40" s="43">
+        <f t="shared" si="3"/>
+        <v>9.2499999999999999E-2</v>
+      </c>
+      <c r="E40" s="4">
+        <f t="shared" si="4"/>
+        <v>33284.46</v>
+      </c>
+      <c r="F40" s="12" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>=SI.ERROR(BUSCARV(C40;J40:K47;2;1);BUSCARV(C40;$M$31:$N$37;2;1))</v>
+      </c>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" s="4">
+        <v>4</v>
+      </c>
+      <c r="C41" s="40">
+        <v>502983</v>
+      </c>
+      <c r="D41" s="43">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="E41" s="4">
+        <f t="shared" si="4"/>
+        <v>50298.3</v>
+      </c>
+      <c r="F41" s="12" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>=SI.ERROR(BUSCARV(C41;J41:K48;2;1);BUSCARV(C41;$M$31:$N$37;2;1))</v>
+      </c>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+    </row>
+    <row r="46" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A46" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A48" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="D48" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="E48" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="J48" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="K48" s="38"/>
+      <c r="M48" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="N48" s="37"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" s="4">
+        <v>2</v>
+      </c>
+      <c r="C49" s="4">
+        <v>120000</v>
+      </c>
+      <c r="D49" s="44"/>
+      <c r="E49" s="4">
+        <v>8400</v>
+      </c>
+      <c r="J49" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="K49" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="M49" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="N49" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" s="4">
+        <v>1</v>
+      </c>
+      <c r="C50" s="4">
+        <v>210921</v>
+      </c>
+      <c r="D50" s="44"/>
+      <c r="E50" s="4">
+        <v>14764.470000000001</v>
+      </c>
+      <c r="J50" s="4">
+        <v>0</v>
+      </c>
+      <c r="K50" s="4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M50" s="4">
+        <v>0</v>
+      </c>
+      <c r="N50" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B51" s="4">
+        <v>1</v>
+      </c>
+      <c r="C51" s="4">
+        <v>100000</v>
+      </c>
+      <c r="D51" s="44"/>
+      <c r="E51" s="4">
+        <v>7000.0000000000009</v>
+      </c>
+      <c r="J51" s="4">
+        <v>5000</v>
+      </c>
+      <c r="K51" s="4">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="M51" s="4">
+        <v>50000</v>
+      </c>
+      <c r="N51" s="4">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B52" s="4">
+        <v>2</v>
+      </c>
+      <c r="C52" s="4">
+        <v>87401</v>
+      </c>
+      <c r="D52" s="44"/>
+      <c r="E52" s="4">
+        <v>5244.0599999999995</v>
+      </c>
+      <c r="J52" s="4">
+        <v>10000</v>
+      </c>
+      <c r="K52" s="4">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="M52" s="4">
+        <v>100000</v>
+      </c>
+      <c r="N52" s="4">
+        <v>7.2499999999999995E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B53" s="4">
+        <v>6</v>
+      </c>
+      <c r="C53" s="4">
+        <v>310983</v>
+      </c>
+      <c r="D53" s="44"/>
+      <c r="E53" s="4">
+        <v>28765.927499999998</v>
+      </c>
+      <c r="J53" s="4">
+        <v>20000</v>
+      </c>
+      <c r="K53" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="M53" s="4">
+        <v>200000</v>
+      </c>
+      <c r="N53" s="4">
+        <v>8.2500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" s="4">
+        <v>3</v>
+      </c>
+      <c r="C54" s="4">
+        <v>43902</v>
+      </c>
+      <c r="D54" s="44"/>
+      <c r="E54" s="4">
+        <v>878.04</v>
+      </c>
+      <c r="J54" s="4">
+        <v>50000</v>
+      </c>
+      <c r="K54" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="M54" s="4">
+        <v>300000</v>
+      </c>
+      <c r="N54" s="4">
+        <v>9.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" s="4">
+        <v>2</v>
+      </c>
+      <c r="C55" s="4">
+        <v>121021</v>
+      </c>
+      <c r="D55" s="44"/>
+      <c r="E55" s="4">
+        <v>8471.4700000000012</v>
+      </c>
+      <c r="J55" s="4">
+        <v>100000</v>
+      </c>
+      <c r="K55" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M55" s="4">
+        <v>500000</v>
+      </c>
+      <c r="N55" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B56" s="4">
+        <v>3</v>
+      </c>
+      <c r="C56" s="4">
+        <v>908</v>
+      </c>
+      <c r="D56" s="44"/>
+      <c r="E56" s="4">
+        <v>18.16</v>
+      </c>
+      <c r="J56" s="4">
+        <v>250000</v>
+      </c>
+      <c r="K56" s="4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B57" s="4">
+        <v>1</v>
+      </c>
+      <c r="C57" s="4">
+        <v>0</v>
+      </c>
+      <c r="D57" s="44"/>
+      <c r="E57" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B58" s="4">
+        <v>4</v>
+      </c>
+      <c r="C58" s="4">
+        <v>359832</v>
+      </c>
+      <c r="D58" s="44"/>
+      <c r="E58" s="4">
+        <v>33284.46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B59" s="4">
+        <v>4</v>
+      </c>
+      <c r="C59" s="4">
+        <v>502983</v>
+      </c>
+      <c r="D59" s="44"/>
+      <c r="E59" s="4">
+        <v>50298.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="M48:N48"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8BB1D6C-BEAB-4376-8D52-1EBE08720090}">
+  <dimension ref="A9:L50"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="9" spans="1:12" ht="21" x14ac:dyDescent="0.4">
+      <c r="A9" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="E12" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="J12" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="L12" s="36" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" s="4">
+        <v>2892</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1771</v>
+      </c>
+      <c r="D13" s="4">
+        <v>4718</v>
+      </c>
+      <c r="E13" s="4">
+        <v>9381</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="K13" s="44"/>
+      <c r="L13" s="44"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" s="4">
+        <v>3380</v>
+      </c>
+      <c r="C14" s="4">
+        <v>4711</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2615</v>
+      </c>
+      <c r="E14" s="4">
+        <v>10706</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="K14" s="44"/>
+      <c r="L14" s="44"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15" s="4">
+        <v>3744</v>
+      </c>
+      <c r="C15" s="4">
+        <v>3223</v>
+      </c>
+      <c r="D15" s="4">
+        <v>5312</v>
+      </c>
+      <c r="E15" s="4">
+        <v>12279</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16" s="4">
+        <v>3221</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2438</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1108</v>
+      </c>
+      <c r="E16" s="4">
+        <v>6767</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="K16" s="44"/>
+      <c r="L16" s="44"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" s="4">
+        <v>4839</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1999</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1994</v>
+      </c>
+      <c r="E17" s="4">
+        <v>8832</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K17" s="44"/>
+      <c r="L17" s="44"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B18" s="4">
+        <v>3767</v>
+      </c>
+      <c r="C18" s="4">
+        <v>5140</v>
+      </c>
+      <c r="D18" s="4">
+        <v>3830</v>
+      </c>
+      <c r="E18" s="4">
+        <v>12737</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="K18" s="44"/>
+      <c r="L18" s="44"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" s="4">
+        <v>5467</v>
+      </c>
+      <c r="C19" s="4">
+        <v>3337</v>
+      </c>
+      <c r="D19" s="4">
+        <v>3232</v>
+      </c>
+      <c r="E19" s="4">
+        <v>12036</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="K19" s="44"/>
+      <c r="L19" s="44"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" s="4">
+        <v>3154</v>
+      </c>
+      <c r="C20" s="4">
+        <v>4895</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1607</v>
+      </c>
+      <c r="E20" s="4">
+        <v>9656</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="K20" s="44"/>
+      <c r="L20" s="44"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1718</v>
+      </c>
+      <c r="C21" s="4">
+        <v>2040</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1563</v>
+      </c>
+      <c r="E21" s="4">
+        <v>5321</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="K21" s="44"/>
+      <c r="L21" s="44"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22" s="4">
+        <v>1548</v>
+      </c>
+      <c r="C22" s="4">
+        <v>1061</v>
+      </c>
+      <c r="D22" s="4">
+        <v>2590</v>
+      </c>
+      <c r="E22" s="4">
+        <v>5199</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="4">
+        <v>5083</v>
+      </c>
+      <c r="C23" s="4">
+        <v>3558</v>
+      </c>
+      <c r="D23" s="4">
+        <v>3960</v>
+      </c>
+      <c r="E23" s="4">
+        <v>12601</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B24" s="4">
+        <v>5753</v>
+      </c>
+      <c r="C24" s="4">
+        <v>2839</v>
+      </c>
+      <c r="D24" s="4">
+        <v>3013</v>
+      </c>
+      <c r="E24" s="4">
+        <v>11605</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B25" s="4">
+        <v>44566</v>
+      </c>
+      <c r="C25" s="4">
+        <v>37012</v>
+      </c>
+      <c r="D25" s="4">
+        <v>35542</v>
+      </c>
+      <c r="E25" s="4">
+        <v>117120</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+    </row>
+    <row r="31" spans="1:12" ht="21" x14ac:dyDescent="0.4">
+      <c r="A31" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="21" x14ac:dyDescent="0.4">
+      <c r="A32" s="6"/>
+    </row>
+    <row r="33" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+      <c r="A33" s="6"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D36" t="s">
+        <v>153</v>
+      </c>
+      <c r="E36" t="s">
+        <v>154</v>
+      </c>
+      <c r="F36" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B37" s="44"/>
+      <c r="D37" t="s">
+        <v>153</v>
+      </c>
+      <c r="E37" t="s">
+        <v>158</v>
+      </c>
+      <c r="F37" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>160</v>
+      </c>
+      <c r="E38" t="s">
+        <v>161</v>
+      </c>
+      <c r="F38" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
+        <v>160</v>
+      </c>
+      <c r="E39" t="s">
+        <v>163</v>
+      </c>
+      <c r="F39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>165</v>
+      </c>
+      <c r="E40" t="s">
+        <v>166</v>
+      </c>
+      <c r="F40" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
+        <v>165</v>
+      </c>
+      <c r="E41" t="s">
+        <v>168</v>
+      </c>
+      <c r="F41" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D42" t="s">
+        <v>170</v>
+      </c>
+      <c r="E42" t="s">
+        <v>171</v>
+      </c>
+      <c r="F42" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>170</v>
+      </c>
+      <c r="E43" t="s">
+        <v>173</v>
+      </c>
+      <c r="F43" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
+        <v>175</v>
+      </c>
+      <c r="E44" t="s">
+        <v>154</v>
+      </c>
+      <c r="F44" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>147</v>
+      </c>
+      <c r="E45" t="s">
+        <v>152</v>
+      </c>
+      <c r="F45" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D46" t="s">
+        <v>147</v>
+      </c>
+      <c r="E46" t="s">
+        <v>177</v>
+      </c>
+      <c r="F46" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
se agrega leccion 5 con desafios
</commit_message>
<xml_diff>
--- a/Lecc4Find/FuncionesBusque.xlsx
+++ b/Lecc4Find/FuncionesBusque.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ReposGit\Excel_InicialDatos\Lecc4Find\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663BF1DB-E8F7-4ED8-A60C-505FAA733495}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA766A1-5C6A-446D-ADF2-194C2A0E7754}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{9ABDD8A0-D50D-4CBA-88BC-C6206BB5B64C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{9ABDD8A0-D50D-4CBA-88BC-C6206BB5B64C}"/>
   </bookViews>
   <sheets>
     <sheet name="1.CondicionesBuscar" sheetId="2" r:id="rId1"/>
@@ -23,6 +23,11 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'03.IndiceCoincir'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'04.buscarx'!#REF!</definedName>
+    <definedName name="CODES">'05.DESAFIO2'!$F$54:$F$65</definedName>
+    <definedName name="MAKES">'05.DESAFIO2'!$D$54:$D$65</definedName>
+    <definedName name="MAYOR3">'05.DESAFIO1'!$M$12:$N$19</definedName>
+    <definedName name="MENOR3">'05.DESAFIO1'!$J$12:$K$20</definedName>
+    <definedName name="MODELS">'05.DESAFIO2'!$E$54:$E$65</definedName>
     <definedName name="Table1">'05.DESAFIO1'!$J$12:$K$20</definedName>
     <definedName name="Table2">'05.DESAFIO1'!$M$12:$N$19</definedName>
   </definedNames>
@@ -66,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="197">
   <si>
     <t>FUNCION</t>
   </si>
@@ -266,12 +271,6 @@
     <t>BASE IMPONIBLE</t>
   </si>
   <si>
-    <t>FRACCION</t>
-  </si>
-  <si>
-    <t>% REBAJA</t>
-  </si>
-  <si>
     <t>% VALOR REDUCCION</t>
   </si>
   <si>
@@ -636,6 +635,33 @@
   </si>
   <si>
     <t>ERET</t>
+  </si>
+  <si>
+    <t>=BUSCARV(VALOR DE BUSQUEDA,MATRIZ, COLUMNA, FALSO/VERDADERO)</t>
+  </si>
+  <si>
+    <t>FRACCION DISMINUIR</t>
+  </si>
+  <si>
+    <t>% RENTA PAGAR</t>
+  </si>
+  <si>
+    <t>IMPUESTO SOBRE BASE</t>
+  </si>
+  <si>
+    <t>INDICE</t>
+  </si>
+  <si>
+    <t>QUE QUIERO TRAER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COINCIDIR </t>
+  </si>
+  <si>
+    <t>COMO LE BUSCO Y EN DONDE LE BUSCO, CON QUE GRADO DE EXACTITUD</t>
+  </si>
+  <si>
+    <t>=INDICE('QUE QUIERO TRAERMATRIZ;NUMERO FILA;NUMERO DE COLUMNA)</t>
   </si>
 </sst>
 </file>
@@ -707,7 +733,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -753,6 +779,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -811,7 +855,7 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -866,19 +910,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="5" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -889,6 +926,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -2087,8 +2151,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1196340</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>36450</xdr:rowOff>
     </xdr:to>
@@ -2156,7 +2220,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>382904</xdr:colOff>
+      <xdr:colOff>93344</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>42760</xdr:rowOff>
     </xdr:to>
@@ -2898,6 +2962,72 @@
             <a:rPr lang="es-EC" sz="2000" b="1" baseline="0"/>
             <a:t> NUMERICOS APROXIMADO INFERIOR</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectángulo: esquinas redondeadas 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CE8272D-2F4F-4F3E-A370-9E0729D0D732}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6339840" y="6217920"/>
+          <a:ext cx="1821180" cy="937260"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100"/>
+            <a:t>REGLA</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" baseline="0"/>
+            <a:t> DE BUSQUEDA APROXIMADA: EL RANGO NUMERICO DEBE ESTAR ORDENADO ASCENDENTE</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-EC" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3530,15 +3660,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>678180</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3553,8 +3683,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="243840" y="6537960"/>
-          <a:ext cx="6918960" cy="1028700"/>
+          <a:off x="99060" y="7414260"/>
+          <a:ext cx="7589520" cy="1028700"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -3590,6 +3720,74 @@
             <a:rPr lang="es-EC" sz="2000" b="1" baseline="0"/>
             <a:t>EL MISMO PODER DE BUSCARV PERO SIN LIMITANTES DE ORDEN DE COLUMNA</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectángulo: esquinas redondeadas 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84B5DC7C-C4C8-487A-B3D5-A4ADBED8EC35}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5791200" y="9029700"/>
+          <a:ext cx="1783080" cy="1043940"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100"/>
+            <a:t>PARA USAR</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" baseline="0"/>
+            <a:t> INDICE Y COINCIDIR LOS RANGOS DEBEN SER IGUALES</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-EC" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -5535,8 +5733,8 @@
   </sheetPr>
   <dimension ref="B9:N65"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView showGridLines="0" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5557,7 +5755,7 @@
         <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="21" x14ac:dyDescent="0.4">
@@ -5606,12 +5804,12 @@
         <v>1</v>
       </c>
       <c r="E16">
-        <f>VLOOKUP(B16,$I$15:$K$21,3,0)</f>
-        <v>34</v>
+        <f>VLOOKUP(B16,$I$15:$K$21,3,1)</f>
+        <v>4565</v>
       </c>
       <c r="F16" t="str">
         <f ca="1">_xlfn.FORMULATEXT(E16)</f>
-        <v>=BUSCARV(B16;$I$15:$K$21;3;0)</v>
+        <v>=BUSCARV(B16;$I$15:$K$21;3;1)</v>
       </c>
       <c r="I16" t="s">
         <v>6</v>
@@ -5669,13 +5867,13 @@
         <f t="shared" ca="1" si="1"/>
         <v>=BUSCARV(B18;$I$15:$K$21;3;0)</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="49">
         <v>3</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="50">
         <v>4565</v>
       </c>
     </row>
@@ -6477,15 +6675,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40B2E87-9AA1-4B2A-8E5A-DDF3639D35E8}">
-  <dimension ref="A16:X46"/>
+  <dimension ref="A16:X52"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.33203125" customWidth="1"/>
@@ -6848,35 +7047,38 @@
         <v>=COINCIDIR(A24;$G$16:$X$16;0)</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
+    <row r="36" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="B38" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="H38" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H38" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="J38" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="9">
         <v>43554</v>
       </c>
-      <c r="B39">
-        <f>VLOOKUP(A39,$H$38:$I$46,2,1)</f>
-        <v>0.23</v>
+      <c r="B39" s="53">
+        <f>(A39-VLOOKUP(A39,$H$38:$J$46,1,1))*VLOOKUP(A39,$H$38:$J$46,2,1)+VLOOKUP(A39,$H$38:$J$46,3,1)</f>
+        <v>2142.9</v>
       </c>
       <c r="C39" t="str">
         <f ca="1">_xlfn.FORMULATEXT(B39)</f>
-        <v>=BUSCARV(A39;$H$38:$I$46;2;1)</v>
+        <v>=(A39-BUSCARV(A39;$H$38:$J$46;1;1))*BUSCARV(A39;$H$38:$J$46;2;1)+BUSCARV(A39;$H$38:$J$46;3;1)</v>
       </c>
       <c r="H39" s="15">
         <v>23334</v>
@@ -6884,18 +7086,21 @@
       <c r="I39" s="14">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="9">
         <v>6656767</v>
       </c>
-      <c r="B40">
-        <f t="shared" ref="B40:B43" si="3">VLOOKUP(A40,$H$38:$I$46,2,1)</f>
-        <v>0.78</v>
+      <c r="B40" s="9">
+        <f t="shared" ref="B40:B43" si="3">(A40-VLOOKUP(A40,$H$38:$J$46,1,1))*VLOOKUP(A40,$H$38:$J$46,2,1)+VLOOKUP(A40,$H$38:$J$46,3,1)</f>
+        <v>5114152.34</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" ref="C40:C43" ca="1" si="4">_xlfn.FORMULATEXT(B40)</f>
-        <v>=BUSCARV(A40;$H$38:$I$46;2;1)</v>
+        <v>=(A40-BUSCARV(A40;$H$38:$J$46;1;1))*BUSCARV(A40;$H$38:$J$46;2;1)+BUSCARV(A40;$H$38:$J$46;3;1)</v>
       </c>
       <c r="H40" s="15">
         <v>34324</v>
@@ -6903,18 +7108,21 @@
       <c r="I40" s="14">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J40">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="9">
         <v>566</v>
       </c>
-      <c r="B41" t="e">
+      <c r="B41" s="9" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>=BUSCARV(A41;$H$38:$I$46;2;1)</v>
+        <v>=(A41-BUSCARV(A41;$H$38:$J$46;1;1))*BUSCARV(A41;$H$38:$J$46;2;1)+BUSCARV(A41;$H$38:$J$46;3;1)</v>
       </c>
       <c r="H41" s="15">
         <v>45314</v>
@@ -6922,18 +7130,21 @@
       <c r="I41" s="14">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J41">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="9">
         <v>4354</v>
       </c>
-      <c r="B42" t="e">
+      <c r="B42" s="9" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>=BUSCARV(A42;$H$38:$I$46;2;1)</v>
+        <v>=(A42-BUSCARV(A42;$H$38:$J$46;1;1))*BUSCARV(A42;$H$38:$J$46;2;1)+BUSCARV(A42;$H$38:$J$46;3;1)</v>
       </c>
       <c r="H42" s="15">
         <v>56304</v>
@@ -6941,18 +7152,21 @@
       <c r="I42" s="14">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J42">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="9">
         <v>675675</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="9">
         <f t="shared" si="3"/>
-        <v>0.78</v>
+        <v>448900.58</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>=BUSCARV(A43;$H$38:$I$46;2;1)</v>
+        <v>=(A43-BUSCARV(A43;$H$38:$J$46;1;1))*BUSCARV(A43;$H$38:$J$46;2;1)+BUSCARV(A43;$H$38:$J$46;3;1)</v>
       </c>
       <c r="H43" s="15">
         <v>67294</v>
@@ -6960,29 +7174,72 @@
       <c r="I43" s="14">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J43">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H44" s="15">
         <v>78284</v>
       </c>
       <c r="I44" s="14">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J44">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H45" s="15">
         <v>89274</v>
       </c>
       <c r="I45" s="14">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C46" s="48" t="s">
+        <v>188</v>
+      </c>
       <c r="H46" s="15">
         <v>100264</v>
       </c>
       <c r="I46" s="14">
         <v>0.78</v>
+      </c>
+      <c r="J46">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B48" s="9">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="15">
+        <v>34324</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" s="51">
+        <f>B48-B49</f>
+        <v>9230</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" s="51">
+        <f>B50*I40</f>
+        <v>2122.9</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" s="52">
+        <f>B51+J40</f>
+        <v>2142.9</v>
       </c>
     </row>
   </sheetData>
@@ -6997,7 +7254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9947BE7E-66F1-44B5-81C4-58BF1FADF6ED}">
   <dimension ref="A9:M97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A74" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A76" workbookViewId="0">
       <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
@@ -7037,13 +7294,13 @@
       <c r="C15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="55" t="s">
         <v>44</v>
       </c>
       <c r="I15" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J15" s="13" t="s">
+      <c r="J15" s="54" t="s">
         <v>43</v>
       </c>
       <c r="K15" s="13" t="s">
@@ -7152,12 +7409,12 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+      <c r="A25" s="56" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -7170,13 +7427,13 @@
       <c r="C27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="55" t="s">
         <v>44</v>
       </c>
       <c r="I27" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J27" s="13" t="s">
+      <c r="J27" s="57" t="s">
         <v>43</v>
       </c>
       <c r="K27" s="13" t="s">
@@ -7187,13 +7444,13 @@
       <c r="A28" t="s">
         <v>6</v>
       </c>
-      <c r="B28">
-        <f>INDEX($H$27:$H$31,MATCH(A28,$J$27:$J$31,0))</f>
+      <c r="B28" s="9">
+        <f>INDEX($H$28:$H$31,MATCH(A28,$J$28:$J$31,0))</f>
         <v>32946</v>
       </c>
       <c r="C28" t="str">
         <f ca="1">_xlfn.FORMULATEXT(B28)</f>
-        <v>=INDICE($H$27:$H$31;COINCIDIR(A28;$J$27:$J$31;0))</v>
+        <v>=INDICE($H$28:$H$31;COINCIDIR(A28;$J$28:$J$31;0))</v>
       </c>
       <c r="H28" s="4">
         <v>32946</v>
@@ -7212,13 +7469,13 @@
       <c r="A29" t="s">
         <v>38</v>
       </c>
-      <c r="B29">
-        <f t="shared" ref="B29:B31" si="2">INDEX($H$27:$H$31,MATCH(A29,$J$27:$J$31,0))</f>
+      <c r="B29" s="9">
+        <f t="shared" ref="B29:B31" si="2">INDEX($H$28:$H$31,MATCH(A29,$J$28:$J$31,0))</f>
         <v>37512</v>
       </c>
       <c r="C29" t="str">
         <f ca="1">_xlfn.FORMULATEXT(B29)</f>
-        <v>=INDICE($H$27:$H$31;COINCIDIR(A29;$J$27:$J$31;0))</v>
+        <v>=INDICE($H$28:$H$31;COINCIDIR(A29;$J$28:$J$31;0))</v>
       </c>
       <c r="H29" s="4">
         <v>37512</v>
@@ -7237,13 +7494,13 @@
       <c r="A30" t="s">
         <v>39</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="9">
         <f t="shared" si="2"/>
         <v>4829</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" ref="C30:C31" ca="1" si="3">_xlfn.FORMULATEXT(B30)</f>
-        <v>=INDICE($H$27:$H$31;COINCIDIR(A30;$J$27:$J$31;0))</v>
+        <v>=INDICE($H$28:$H$31;COINCIDIR(A30;$J$28:$J$31;0))</v>
       </c>
       <c r="H30" s="4">
         <v>4829</v>
@@ -7262,13 +7519,13 @@
       <c r="A31" t="s">
         <v>40</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="9">
         <f t="shared" si="2"/>
         <v>68836</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>=INDICE($H$27:$H$31;COINCIDIR(A31;$J$27:$J$31;0))</v>
+        <v>=INDICE($H$28:$H$31;COINCIDIR(A31;$J$28:$J$31;0))</v>
       </c>
       <c r="H31" s="4">
         <v>68836</v>
@@ -7283,42 +7540,55 @@
         <v>31194</v>
       </c>
     </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B34" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B35" t="s">
+        <v>195</v>
+      </c>
+    </row>
     <row r="42" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="B42" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B43" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C43" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B44" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C44" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B47" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>37</v>
+      <c r="C47" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>0</v>
+      <c r="E47" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="J47" s="13" t="s">
         <v>44</v>
@@ -7334,24 +7604,28 @@
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>2</v>
+      <c r="A48" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(D48)</f>
+        <v>=INDICE($J$47:$J$53;COINCIDIR(E48;$L$47:$L$53;0))</v>
       </c>
       <c r="B48">
         <v>2</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <f>INDEX($J$47:$J$53,MATCH(E48,$L$47:$L$53,0))</f>
+        <v>32946</v>
+      </c>
+      <c r="E48" t="s">
         <v>6</v>
       </c>
-      <c r="D48">
-        <f>INDEX($K$48:$K$53,MATCH(C48,$L$48:$L$53,0))</f>
-        <v>43751</v>
-      </c>
-      <c r="E48" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(D48)</f>
-        <v>=INDICE($K$48:$K$53;COINCIDIR(C48;$L$48:$L$53;0))</v>
-      </c>
-      <c r="J48" s="4">
+      <c r="F48">
+        <f>INDEX($J$48:$J$53,MATCH(E48,$L$48:$L$53,0))</f>
+        <v>32946</v>
+      </c>
+      <c r="J48" s="37">
         <v>32946</v>
       </c>
       <c r="K48" s="4">
@@ -7365,24 +7639,28 @@
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <v>5</v>
+      <c r="A49" t="str">
+        <f t="shared" ref="A49:A53" ca="1" si="4">_xlfn.FORMULATEXT(D49)</f>
+        <v>=INDICE($J$47:$J$53;COINCIDIR(E49;$L$47:$L$53;0))</v>
       </c>
       <c r="B49">
         <v>4</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49">
+        <v>4</v>
+      </c>
+      <c r="D49">
+        <f t="shared" ref="D49:D53" si="5">INDEX($J$47:$J$53,MATCH(E49,$L$47:$L$53,0))</f>
+        <v>37512</v>
+      </c>
+      <c r="E49" t="s">
         <v>38</v>
       </c>
-      <c r="D49">
-        <f t="shared" ref="D49:D53" si="4">INDEX($K$48:$K$53,MATCH(C49,$L$48:$L$53,0))</f>
-        <v>43254</v>
-      </c>
-      <c r="E49" t="str">
-        <f t="shared" ref="E49:E53" ca="1" si="5">_xlfn.FORMULATEXT(D49)</f>
-        <v>=INDICE($K$48:$K$53;COINCIDIR(C49;$L$48:$L$53;0))</v>
-      </c>
-      <c r="J49" s="4">
+      <c r="F49">
+        <f t="shared" ref="F49:F53" si="6">INDEX($J$48:$J$53,MATCH(E49,$L$48:$L$53,0))</f>
+        <v>37512</v>
+      </c>
+      <c r="J49" s="37">
         <v>37512</v>
       </c>
       <c r="K49" s="4">
@@ -7396,24 +7674,28 @@
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <v>3</v>
+      <c r="A50" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>=INDICE($J$47:$J$53;COINCIDIR(E50;$L$47:$L$53;0))</v>
       </c>
       <c r="B50">
         <v>8</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50">
+        <v>8</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="5"/>
+        <v>4829</v>
+      </c>
+      <c r="E50" t="s">
         <v>39</v>
       </c>
-      <c r="D50">
-        <f t="shared" si="4"/>
-        <v>62487</v>
-      </c>
-      <c r="E50" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>=INDICE($K$48:$K$53;COINCIDIR(C50;$L$48:$L$53;0))</v>
-      </c>
-      <c r="J50" s="4">
+      <c r="F50">
+        <f t="shared" si="6"/>
+        <v>4829</v>
+      </c>
+      <c r="J50" s="37">
         <v>4829</v>
       </c>
       <c r="K50" s="4">
@@ -7427,24 +7709,28 @@
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <v>5</v>
+      <c r="A51" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>=INDICE($J$47:$J$53;COINCIDIR(E51;$L$47:$L$53;0))</v>
       </c>
       <c r="B51">
         <v>5</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51">
+        <v>5</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="5"/>
+        <v>37512</v>
+      </c>
+      <c r="E51" t="s">
         <v>40</v>
       </c>
-      <c r="D51">
-        <f t="shared" si="4"/>
-        <v>43254</v>
-      </c>
-      <c r="E51" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>=INDICE($K$48:$K$53;COINCIDIR(C51;$L$48:$L$53;0))</v>
-      </c>
-      <c r="J51" s="4">
+      <c r="F51">
+        <f t="shared" si="6"/>
+        <v>37512</v>
+      </c>
+      <c r="J51" s="37">
         <v>37512</v>
       </c>
       <c r="K51" s="4">
@@ -7458,62 +7744,70 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <v>4</v>
+      <c r="A52" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>=INDICE($J$47:$J$53;COINCIDIR(E52;$L$47:$L$53;0))</v>
       </c>
       <c r="B52">
         <v>4</v>
       </c>
-      <c r="C52" t="s">
-        <v>75</v>
+      <c r="C52">
+        <v>4</v>
       </c>
       <c r="D52">
-        <f t="shared" si="4"/>
-        <v>62487</v>
-      </c>
-      <c r="E52" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>=INDICE($K$48:$K$53;COINCIDIR(C52;$L$48:$L$53;0))</v>
-      </c>
-      <c r="J52" s="4">
+        <f t="shared" si="5"/>
+        <v>4829</v>
+      </c>
+      <c r="E52" t="s">
+        <v>73</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="6"/>
+        <v>4829</v>
+      </c>
+      <c r="J52" s="37">
         <v>4829</v>
       </c>
       <c r="K52" s="4">
         <v>62487</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M52" s="4">
         <v>22196</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <v>8</v>
+      <c r="A53" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>=INDICE($J$47:$J$53;COINCIDIR(E53;$L$47:$L$53;0))</v>
       </c>
       <c r="B53">
         <v>8</v>
       </c>
-      <c r="C53" t="s">
-        <v>76</v>
+      <c r="C53">
+        <v>8</v>
       </c>
       <c r="D53">
-        <f t="shared" si="4"/>
-        <v>43254</v>
-      </c>
-      <c r="E53" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>=INDICE($K$48:$K$53;COINCIDIR(C53;$L$48:$L$53;0))</v>
-      </c>
-      <c r="J53" s="4">
+        <f t="shared" si="5"/>
+        <v>68836</v>
+      </c>
+      <c r="E53" t="s">
+        <v>74</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="6"/>
+        <v>68836</v>
+      </c>
+      <c r="J53" s="37">
         <v>68836</v>
       </c>
       <c r="K53" s="4">
         <v>43254</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M53" s="4">
         <v>22196</v>
@@ -7521,24 +7815,24 @@
     </row>
     <row r="57" spans="1:13" ht="21" x14ac:dyDescent="0.4">
       <c r="C57" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B59" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D59" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C59" s="16" t="s">
+      <c r="F59" t="s">
         <v>96</v>
       </c>
-      <c r="D59" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="F59" t="s">
-        <v>98</v>
-      </c>
       <c r="H59" s="4" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
@@ -7549,21 +7843,21 @@
         <v>0</v>
       </c>
       <c r="D60" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B61">
+      <c r="B61" s="58">
         <v>9</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="58">
         <v>0.33300000000000002</v>
       </c>
-      <c r="D61" t="s">
-        <v>81</v>
+      <c r="D61" s="58" t="s">
+        <v>79</v>
       </c>
       <c r="F61" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H61" s="4" t="str">
         <f>VLOOKUP($H$59,$B$59:$D$74,2)</f>
@@ -7582,10 +7876,10 @@
         <v>0.33300000000000002</v>
       </c>
       <c r="D62" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F62" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H62" s="4" t="str">
         <f>VLOOKUP($H$59,$B$59:$D$74,1)</f>
@@ -7604,7 +7898,7 @@
         <v>0.28599999999999998</v>
       </c>
       <c r="D63" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
@@ -7615,7 +7909,7 @@
         <v>0.313</v>
       </c>
       <c r="D64" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
@@ -7626,18 +7920,18 @@
         <v>0.217</v>
       </c>
       <c r="D65" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F65" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H65" s="4">
-        <f>INDEX($C$60:$C$74,MATCH($H$59,$D$60:$D$74,0))</f>
-        <v>0.3</v>
+        <f>INDEX($C$60:$C$74,MATCH(H59,$D$60:$D$74,0))</f>
+        <v>0.33300000000000002</v>
       </c>
       <c r="J65" t="str">
         <f ca="1">_xlfn.FORMULATEXT(H65)</f>
-        <v>=INDICE($C$60:$C$74;COINCIDIR($H$59;$D$60:$D$74;0))</v>
+        <v>=INDICE($C$60:$C$74;COINCIDIR(H59;$D$60:$D$74;0))</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
@@ -7648,18 +7942,18 @@
         <v>0.33300000000000002</v>
       </c>
       <c r="D66" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F66" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H66" s="4">
-        <f>INDEX($B$60:$B$74,MATCH($H$59,$D$60:$D$74,0))</f>
-        <v>30</v>
+        <f>INDEX($B$60:$B$74,MATCH(H59,$D$60:$D$74,0))</f>
+        <v>9</v>
       </c>
       <c r="J66" t="str">
         <f ca="1">_xlfn.FORMULATEXT(H66)</f>
-        <v>=INDICE($B$60:$B$74;COINCIDIR($H$59;$D$60:$D$74;0))</v>
+        <v>=INDICE($B$60:$B$74;COINCIDIR(H59;$D$60:$D$74;0))</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
@@ -7670,7 +7964,7 @@
         <v>0.16</v>
       </c>
       <c r="D67" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
@@ -7681,18 +7975,18 @@
         <v>0.32100000000000001</v>
       </c>
       <c r="D68" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B69">
+      <c r="B69" s="58">
         <v>30</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="58">
         <v>0.3</v>
       </c>
-      <c r="D69" t="s">
-        <v>89</v>
+      <c r="D69" s="58" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
@@ -7703,7 +7997,7 @@
         <v>0.13900000000000001</v>
       </c>
       <c r="D70" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
@@ -7714,7 +8008,7 @@
         <v>0.39</v>
       </c>
       <c r="D71" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
@@ -7725,7 +8019,10 @@
         <v>0.186</v>
       </c>
       <c r="D72" t="s">
-        <v>92</v>
+        <v>90</v>
+      </c>
+      <c r="G72" s="48" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
@@ -7736,7 +8033,7 @@
         <v>0.34100000000000003</v>
       </c>
       <c r="D73" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
@@ -7747,12 +8044,12 @@
         <v>0.33300000000000002</v>
       </c>
       <c r="D74" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
@@ -7760,73 +8057,56 @@
         <v>2</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="H80" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="H80" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="I80" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="J80" s="2" t="s">
-        <v>182</v>
+      <c r="I80" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J80" s="59" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B81" cm="1">
-        <f t="array" ref="B81">INDEX($H$81:$J$81,,MATCH(B$80,$H$80:$J$80,0))</f>
+        <f t="array" ref="B81">INDEX($H$81:$J$81,,MATCH(B80,$H$80:$J$80,0))</f>
         <v>1234</v>
       </c>
       <c r="C81" cm="1">
-        <f t="array" ref="C81">INDEX($H$81:$J$81,,MATCH(C$80,$H$80:$J$80,0))</f>
+        <f t="array" ref="C81">INDEX($H$81:$J$81,,MATCH(C80,$H$80:$J$80,0))</f>
         <v>456</v>
       </c>
       <c r="D81" cm="1">
-        <f t="array" ref="D81">INDEX($H$81:$J$81,,MATCH(D$80,$H$80:$J$80,0))</f>
+        <f t="array" ref="D81">INDEX($H$81:$J$81,,MATCH(D80,$H$80:$J$80,0))</f>
         <v>567</v>
       </c>
-      <c r="H81">
+      <c r="H81" s="4">
         <v>1234</v>
       </c>
-      <c r="I81">
+      <c r="I81" s="4">
         <v>456</v>
       </c>
-      <c r="J81">
+      <c r="J81" s="4">
         <v>567</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B82" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B81)</f>
-        <v>=INDICE($H$81:$J$81;;COINCIDIR(B$80;$H$80:$J$80;0))</v>
-      </c>
-      <c r="C82" t="str">
-        <f t="shared" ref="C82:D82" ca="1" si="6">_xlfn.FORMULATEXT(C81)</f>
-        <v>=INDICE($H$81:$J$81;;COINCIDIR(C$80;$H$80:$J$80;0))</v>
-      </c>
-      <c r="D82" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>=INDICE($H$81:$J$81;;COINCIDIR(D$80;$H$80:$J$80;0))</v>
-      </c>
-    </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
+      <c r="A93" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>5</v>
@@ -7835,10 +8115,10 @@
         <v>2</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K93" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.3">
@@ -7850,23 +8130,19 @@
         <v>ASD</v>
       </c>
       <c r="C94">
-        <f t="shared" ref="C94:D97" si="7">INDEX($I$94:$K$97,MATCH($A94,$H$94:$H$97,0),MATCH(C$93,$I$93:$K$93,0))</f>
+        <f>INDEX($I$94:$K$97,MATCH($A94,$H$94:$H$97,0),MATCH(C$93,$I$93:$K$93,0))</f>
         <v>324</v>
-      </c>
-      <c r="D94">
-        <f t="shared" si="7"/>
-        <v>56</v>
       </c>
       <c r="H94">
         <v>123</v>
       </c>
-      <c r="I94" t="s">
-        <v>184</v>
-      </c>
-      <c r="J94">
+      <c r="I94" s="60" t="s">
+        <v>182</v>
+      </c>
+      <c r="J94" s="60">
         <v>324</v>
       </c>
-      <c r="K94">
+      <c r="K94" s="60">
         <v>56</v>
       </c>
     </row>
@@ -7875,27 +8151,23 @@
         <v>1234</v>
       </c>
       <c r="B95" t="str">
-        <f t="shared" ref="B95:B97" si="8">INDEX($I$94:$K$97,MATCH($A95,$H$94:$H$97,0),MATCH(B$93,$I$93:$K$93,0))</f>
+        <f t="shared" ref="B95:C97" si="7">INDEX($I$94:$K$97,MATCH($A95,$H$94:$H$97,0),MATCH(B$93,$I$93:$K$93,0))</f>
         <v>DS</v>
       </c>
       <c r="C95">
         <f t="shared" si="7"/>
         <v>344</v>
       </c>
-      <c r="D95">
-        <f t="shared" si="7"/>
-        <v>765</v>
-      </c>
       <c r="H95">
         <v>1234</v>
       </c>
-      <c r="I95" t="s">
-        <v>185</v>
-      </c>
-      <c r="J95">
+      <c r="I95" s="60" t="s">
+        <v>183</v>
+      </c>
+      <c r="J95" s="60">
         <v>344</v>
       </c>
-      <c r="K95">
+      <c r="K95" s="60">
         <v>765</v>
       </c>
     </row>
@@ -7904,27 +8176,23 @@
         <v>12345</v>
       </c>
       <c r="B96" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>DFS</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="7"/>
         <v>EFEW</v>
       </c>
-      <c r="D96">
-        <f t="shared" si="7"/>
-        <v>453</v>
-      </c>
       <c r="H96">
         <v>12345</v>
       </c>
-      <c r="I96" t="s">
+      <c r="I96" s="60" t="s">
+        <v>184</v>
+      </c>
+      <c r="J96" s="60" t="s">
         <v>186</v>
       </c>
-      <c r="J96" t="s">
-        <v>188</v>
-      </c>
-      <c r="K96">
+      <c r="K96" s="60">
         <v>453</v>
       </c>
     </row>
@@ -7933,27 +8201,23 @@
         <v>123445</v>
       </c>
       <c r="B97" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>FGD</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="7"/>
         <v>ERET</v>
       </c>
-      <c r="D97">
-        <f t="shared" si="7"/>
-        <v>23</v>
-      </c>
       <c r="H97">
         <v>123445</v>
       </c>
-      <c r="I97" t="s">
+      <c r="I97" s="60" t="s">
+        <v>185</v>
+      </c>
+      <c r="J97" s="60" t="s">
         <v>187</v>
       </c>
-      <c r="J97" t="s">
-        <v>189</v>
-      </c>
-      <c r="K97">
+      <c r="K97" s="60">
         <v>23</v>
       </c>
     </row>
@@ -7969,7 +8233,7 @@
   <dimension ref="B10:J25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7985,19 +8249,19 @@
   <sheetData>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="F10" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="F10" t="s">
-        <v>98</v>
-      </c>
       <c r="H10" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
@@ -8008,7 +8272,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
@@ -8019,10 +8283,10 @@
         <v>0.33300000000000002</v>
       </c>
       <c r="D12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H12" s="4">
         <f>_xlfn.XLOOKUP($H$10,$D$11:$D$25,$C$11:$C$25,,0)</f>
@@ -8041,10 +8305,10 @@
         <v>0.33300000000000002</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H13" s="4">
         <f>_xlfn.XLOOKUP($H$10,$D$11:$D$25,$B$11:$B$25,,0)</f>
@@ -8063,7 +8327,7 @@
         <v>0.28599999999999998</v>
       </c>
       <c r="D14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
@@ -8074,7 +8338,7 @@
         <v>0.313</v>
       </c>
       <c r="D15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
@@ -8085,10 +8349,10 @@
         <v>0.217</v>
       </c>
       <c r="D16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>24</v>
       </c>
@@ -8096,10 +8360,10 @@
         <v>0.33300000000000002</v>
       </c>
       <c r="D17" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>25</v>
       </c>
@@ -8107,10 +8371,14 @@
         <v>0.16</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="H18">
+        <f>_xlfn.XLOOKUP(H10,$D$11:$D$25,$B$11:$B$25,"NO HAY",0)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>28</v>
       </c>
@@ -8118,10 +8386,10 @@
         <v>0.32100000000000001</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>30</v>
       </c>
@@ -8129,10 +8397,10 @@
         <v>0.3</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>36</v>
       </c>
@@ -8140,10 +8408,10 @@
         <v>0.13900000000000001</v>
       </c>
       <c r="D21" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>41</v>
       </c>
@@ -8151,10 +8419,10 @@
         <v>0.39</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>43</v>
       </c>
@@ -8162,10 +8430,10 @@
         <v>0.186</v>
       </c>
       <c r="D23" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>44</v>
       </c>
@@ -8173,10 +8441,10 @@
         <v>0.34100000000000003</v>
       </c>
       <c r="D24" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>51</v>
       </c>
@@ -8184,7 +8452,7 @@
         <v>0.33300000000000002</v>
       </c>
       <c r="D25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -8198,8 +8466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97223706-25BC-4B5C-AFEB-83702A354A86}">
   <dimension ref="A9:N59"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8215,47 +8483,47 @@
   <sheetData>
     <row r="9" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="D12" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="C12" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>116</v>
-      </c>
       <c r="E12" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I12" s="20"/>
       <c r="J12" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K12" s="22"/>
       <c r="L12" s="23"/>
       <c r="M12" s="21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="N12" s="22"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B13" s="25">
         <v>2</v>
@@ -8264,37 +8532,37 @@
         <v>120000</v>
       </c>
       <c r="D13" s="27">
-        <f>VLOOKUP(C13,IF(B13&lt;3,Table1,Table2),2)</f>
+        <f>VLOOKUP(C13,IF(B13&gt;=3,MAYOR3,MENOR3),2,1)</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E13" s="26">
         <f>C13*D13</f>
         <v>8400</v>
       </c>
-      <c r="F13" s="41" t="str">
+      <c r="F13" s="38" t="str">
         <f ca="1">_xlfn.FORMULATEXT(D13)</f>
-        <v>=BUSCARV(C13;SI(B13&lt;3;Table1;Table2);2)</v>
-      </c>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
+        <v>=BUSCARV(C13;SI(B13&gt;=3;MAYOR3;MENOR3);2;1)</v>
+      </c>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
       <c r="I13" s="20"/>
       <c r="J13" s="28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K13" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="L13" s="20"/>
       <c r="M13" s="28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="N13" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B14" s="30">
         <v>1</v>
@@ -8302,36 +8570,36 @@
       <c r="C14" s="31">
         <v>210921</v>
       </c>
-      <c r="D14" s="32">
-        <f t="shared" ref="D14:D23" si="0">VLOOKUP(C14,IF(B14&lt;3,Table1,Table2),2)</f>
+      <c r="D14" s="27">
+        <f>VLOOKUP(C14,IF(B14&gt;=3,MAYOR3,MENOR3),2,1)</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E14" s="31">
-        <f t="shared" ref="E14:E23" si="1">C14*D14</f>
+        <f t="shared" ref="E14:E23" si="0">C14*D14</f>
         <v>14764.470000000001</v>
       </c>
-      <c r="F14" s="41" t="str">
-        <f t="shared" ref="F14:F23" ca="1" si="2">_xlfn.FORMULATEXT(D14)</f>
-        <v>=BUSCARV(C14;SI(B14&lt;3;Table1;Table2);2)</v>
-      </c>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="J14" s="33">
+      <c r="F14" s="38" t="str">
+        <f t="shared" ref="F14:F23" ca="1" si="1">_xlfn.FORMULATEXT(D14)</f>
+        <v>=BUSCARV(C14;SI(B14&gt;=3;MAYOR3;MENOR3);2;1)</v>
+      </c>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="J14" s="32">
         <v>0</v>
       </c>
-      <c r="K14" s="34">
+      <c r="K14" s="33">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M14" s="33">
+      <c r="M14" s="32">
         <v>0</v>
       </c>
-      <c r="N14" s="34">
+      <c r="N14" s="33">
         <v>0.02</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B15" s="30">
         <v>1</v>
@@ -8339,37 +8607,37 @@
       <c r="C15" s="31">
         <v>100000</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="27">
+        <f>VLOOKUP(C15,IF(B15&gt;=3,MAYOR3,MENOR3),2,1)</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E15" s="31">
         <f t="shared" si="0"/>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E15" s="31">
-        <f t="shared" si="1"/>
         <v>7000.0000000000009</v>
       </c>
-      <c r="F15" s="41" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>=BUSCARV(C15;SI(B15&lt;3;Table1;Table2);2)</v>
-      </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="J15" s="33">
+      <c r="F15" s="38" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=BUSCARV(C15;SI(B15&gt;=3;MAYOR3;MENOR3);2;1)</v>
+      </c>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="J15" s="32">
         <f>J14+5000</f>
         <v>5000</v>
       </c>
-      <c r="K15" s="34">
+      <c r="K15" s="33">
         <v>3.2500000000000001E-2</v>
       </c>
-      <c r="M15" s="33">
+      <c r="M15" s="32">
         <v>50000</v>
       </c>
-      <c r="N15" s="34">
+      <c r="N15" s="33">
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B16" s="30">
         <v>2</v>
@@ -8377,37 +8645,37 @@
       <c r="C16" s="31">
         <v>87401</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="27">
+        <f>VLOOKUP(C16,IF(B16&gt;=3,MAYOR3,MENOR3),2,1)</f>
+        <v>0.06</v>
+      </c>
+      <c r="E16" s="31">
         <f t="shared" si="0"/>
-        <v>0.06</v>
-      </c>
-      <c r="E16" s="31">
-        <f t="shared" si="1"/>
         <v>5244.0599999999995</v>
       </c>
-      <c r="F16" s="41" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>=BUSCARV(C16;SI(B16&lt;3;Table1;Table2);2)</v>
-      </c>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="J16" s="33">
+      <c r="F16" s="38" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=BUSCARV(C16;SI(B16&gt;=3;MAYOR3;MENOR3);2;1)</v>
+      </c>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="J16" s="32">
         <f>J15+5000</f>
         <v>10000</v>
       </c>
-      <c r="K16" s="34">
+      <c r="K16" s="33">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="M16" s="33">
+      <c r="M16" s="32">
         <v>100000</v>
       </c>
-      <c r="N16" s="34">
+      <c r="N16" s="33">
         <v>7.2499999999999995E-2</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B17" s="30">
         <v>6</v>
@@ -8415,36 +8683,36 @@
       <c r="C17" s="31">
         <v>310983</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="27">
+        <f>VLOOKUP(C17,IF(B17&gt;=3,MAYOR3,MENOR3),2,1)</f>
+        <v>9.2499999999999999E-2</v>
+      </c>
+      <c r="E17" s="31">
         <f t="shared" si="0"/>
-        <v>9.2499999999999999E-2</v>
-      </c>
-      <c r="E17" s="31">
-        <f t="shared" si="1"/>
         <v>28765.927499999998</v>
       </c>
-      <c r="F17" s="41" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>=BUSCARV(C17;SI(B17&lt;3;Table1;Table2);2)</v>
-      </c>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="J17" s="33">
+      <c r="F17" s="38" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=BUSCARV(C17;SI(B17&gt;=3;MAYOR3;MENOR3);2;1)</v>
+      </c>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="J17" s="32">
         <v>20000</v>
       </c>
-      <c r="K17" s="34">
+      <c r="K17" s="33">
         <v>0.05</v>
       </c>
-      <c r="M17" s="33">
+      <c r="M17" s="32">
         <v>200000</v>
       </c>
-      <c r="N17" s="34">
+      <c r="N17" s="33">
         <v>8.2500000000000004E-2</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B18" s="30">
         <v>3</v>
@@ -8452,36 +8720,36 @@
       <c r="C18" s="31">
         <v>43902</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="27">
+        <f>VLOOKUP(C18,IF(B18&gt;=3,MAYOR3,MENOR3),2,1)</f>
+        <v>0.02</v>
+      </c>
+      <c r="E18" s="31">
         <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-      <c r="E18" s="31">
-        <f t="shared" si="1"/>
         <v>878.04</v>
       </c>
-      <c r="F18" s="41" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>=BUSCARV(C18;SI(B18&lt;3;Table1;Table2);2)</v>
-      </c>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="J18" s="33">
+      <c r="F18" s="38" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=BUSCARV(C18;SI(B18&gt;=3;MAYOR3;MENOR3);2;1)</v>
+      </c>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="J18" s="32">
         <v>50000</v>
       </c>
-      <c r="K18" s="34">
+      <c r="K18" s="33">
         <v>0.06</v>
       </c>
-      <c r="M18" s="33">
+      <c r="M18" s="32">
         <v>300000</v>
       </c>
-      <c r="N18" s="34">
+      <c r="N18" s="33">
         <v>9.2499999999999999E-2</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B19" s="30">
         <v>2</v>
@@ -8489,36 +8757,36 @@
       <c r="C19" s="31">
         <v>121021</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="27">
+        <f>VLOOKUP(C19,IF(B19&gt;=3,MAYOR3,MENOR3),2,1)</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E19" s="31">
         <f t="shared" si="0"/>
+        <v>8471.4700000000012</v>
+      </c>
+      <c r="F19" s="38" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=BUSCARV(C19;SI(B19&gt;=3;MAYOR3;MENOR3);2;1)</v>
+      </c>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="J19" s="32">
+        <v>100000</v>
+      </c>
+      <c r="K19" s="33">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E19" s="31">
-        <f t="shared" si="1"/>
-        <v>8471.4700000000012</v>
-      </c>
-      <c r="F19" s="41" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>=BUSCARV(C19;SI(B19&lt;3;Table1;Table2);2)</v>
-      </c>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
-      <c r="J19" s="33">
-        <v>100000</v>
-      </c>
-      <c r="K19" s="34">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="M19" s="33">
+      <c r="M19" s="32">
         <v>500000</v>
       </c>
-      <c r="N19" s="34">
+      <c r="N19" s="33">
         <v>0.1</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B20" s="30">
         <v>3</v>
@@ -8526,30 +8794,30 @@
       <c r="C20" s="31">
         <v>908</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="27">
+        <f>VLOOKUP(C20,IF(B20&gt;=3,MAYOR3,MENOR3),2,1)</f>
+        <v>0.02</v>
+      </c>
+      <c r="E20" s="31">
         <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-      <c r="E20" s="31">
-        <f t="shared" si="1"/>
         <v>18.16</v>
       </c>
-      <c r="F20" s="41" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>=BUSCARV(C20;SI(B20&lt;3;Table1;Table2);2)</v>
-      </c>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="J20" s="33">
+      <c r="F20" s="38" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=BUSCARV(C20;SI(B20&gt;=3;MAYOR3;MENOR3);2;1)</v>
+      </c>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="J20" s="32">
         <v>250000</v>
       </c>
-      <c r="K20" s="34">
+      <c r="K20" s="33">
         <v>0.08</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B21" s="30">
         <v>1</v>
@@ -8557,24 +8825,24 @@
       <c r="C21" s="31">
         <v>0</v>
       </c>
-      <c r="D21" s="32">
+      <c r="D21" s="27">
+        <f>VLOOKUP(C21,IF(B21&gt;=3,MAYOR3,MENOR3),2,1)</f>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E21" s="31">
         <f t="shared" si="0"/>
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="E21" s="31">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F21" s="41" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>=BUSCARV(C21;SI(B21&lt;3;Table1;Table2);2)</v>
-      </c>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
+      <c r="F21" s="38" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=BUSCARV(C21;SI(B21&gt;=3;MAYOR3;MENOR3);2;1)</v>
+      </c>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B22" s="30">
         <v>4</v>
@@ -8582,24 +8850,24 @@
       <c r="C22" s="31">
         <v>359832</v>
       </c>
-      <c r="D22" s="32">
+      <c r="D22" s="27">
+        <f>VLOOKUP(C22,IF(B22&gt;=3,MAYOR3,MENOR3),2,1)</f>
+        <v>9.2499999999999999E-2</v>
+      </c>
+      <c r="E22" s="31">
         <f t="shared" si="0"/>
-        <v>9.2499999999999999E-2</v>
-      </c>
-      <c r="E22" s="31">
-        <f t="shared" si="1"/>
         <v>33284.46</v>
       </c>
-      <c r="F22" s="41" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>=BUSCARV(C22;SI(B22&lt;3;Table1;Table2);2)</v>
-      </c>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
+      <c r="F22" s="38" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=BUSCARV(C22;SI(B22&gt;=3;MAYOR3;MENOR3);2;1)</v>
+      </c>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B23" s="30">
         <v>4</v>
@@ -8607,71 +8875,71 @@
       <c r="C23" s="31">
         <v>502983</v>
       </c>
-      <c r="D23" s="32">
+      <c r="D23" s="27">
+        <f>VLOOKUP(C23,IF(B23&gt;=3,MAYOR3,MENOR3),2,1)</f>
+        <v>0.1</v>
+      </c>
+      <c r="E23" s="31">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="E23" s="31">
-        <f t="shared" si="1"/>
         <v>50298.3</v>
       </c>
-      <c r="F23" s="41" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>=BUSCARV(C23;SI(B23&lt;3;Table1;Table2);2)</v>
-      </c>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
+      <c r="F23" s="38" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=BUSCARV(C23;SI(B23&gt;=3;MAYOR3;MENOR3);2;1)</v>
+      </c>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="B30" s="45" t="s">
+      <c r="D30" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="C30" s="45" t="s">
+      <c r="E30" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="J30" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="D30" s="45" t="s">
+      <c r="K30" s="44"/>
+      <c r="M30" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="E30" s="45" t="s">
-        <v>100</v>
-      </c>
-      <c r="J30" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="K30" s="38"/>
-      <c r="M30" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="N30" s="37"/>
+      <c r="N30" s="45"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B31" s="4">
         <v>2</v>
       </c>
-      <c r="C31" s="40">
+      <c r="C31" s="37">
         <v>120000</v>
       </c>
-      <c r="D31" s="43">
-        <f>IFERROR(VLOOKUP(C31,J31:K38,2,1),VLOOKUP(C31,$M$31:$N$37,2,1))</f>
+      <c r="D31" s="40">
+        <f>IFERROR(VLOOKUP(C31,$J$31:$K$38,2,1),VLOOKUP(C31,$M$31:$N$37,2,1))</f>
         <v>0.08</v>
       </c>
       <c r="E31" s="4">
@@ -8680,109 +8948,107 @@
       </c>
       <c r="F31" s="12" t="str">
         <f ca="1">_xlfn.FORMULATEXT(D31)</f>
-        <v>=SI.ERROR(BUSCARV(C31;J31:K38;2;1);BUSCARV(C31;$M$31:$N$37;2;1))</v>
+        <v>=SI.ERROR(BUSCARV(C31;$J$31:$K$38;2;1);BUSCARV(C31;$M$31:$N$37;2;1))</v>
       </c>
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
-      <c r="J31" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="K31" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="M31" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="N31" s="36" t="s">
-        <v>102</v>
+      <c r="J31" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="K31" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="M31" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="N31" s="35" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B32" s="4">
         <v>1</v>
       </c>
-      <c r="C32" s="40">
+      <c r="C32" s="37">
         <v>210921</v>
       </c>
-      <c r="D32" s="43">
-        <f t="shared" ref="D32:D41" si="3">IFERROR(VLOOKUP(C32,J32:K39,2,1),VLOOKUP(C32,$M$31:$N$37,2,1))</f>
+      <c r="D32" s="40">
+        <f t="shared" ref="D32:D41" si="2">IFERROR(VLOOKUP(C32,$J$31:$K$38,2,1),VLOOKUP(C32,$M$31:$N$37,2,1))</f>
         <v>0.08</v>
       </c>
       <c r="E32" s="4">
-        <f t="shared" ref="E32:E41" si="4">C32*D32</f>
+        <f>C32*D32</f>
         <v>16873.68</v>
       </c>
       <c r="F32" s="12" t="str">
-        <f t="shared" ref="F32:F41" ca="1" si="5">_xlfn.FORMULATEXT(D32)</f>
-        <v>=SI.ERROR(BUSCARV(C32;J32:K39;2;1);BUSCARV(C32;$M$31:$N$37;2;1))</v>
+        <f t="shared" ref="F32:F41" ca="1" si="3">_xlfn.FORMULATEXT(D32)</f>
+        <v>=SI.ERROR(BUSCARV(C32;$J$31:$K$38;2;1);BUSCARV(C32;$M$31:$N$37;2;1))</v>
       </c>
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
-      <c r="J32" s="40">
+      <c r="J32" s="37"/>
+      <c r="K32" s="36">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M32" s="37">
         <v>0</v>
       </c>
-      <c r="K32" s="39">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="M32" s="40">
-        <v>0</v>
-      </c>
-      <c r="N32" s="39">
+      <c r="N32" s="36">
         <v>0.02</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B33" s="4">
         <v>1</v>
       </c>
-      <c r="C33" s="40">
+      <c r="C33" s="37">
         <v>100000</v>
       </c>
-      <c r="D33" s="43">
-        <f t="shared" si="3"/>
+      <c r="D33" s="40">
+        <f t="shared" si="2"/>
         <v>0.08</v>
       </c>
       <c r="E33" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="E32:E41" si="4">C33*D33</f>
         <v>8000</v>
       </c>
       <c r="F33" s="12" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>=SI.ERROR(BUSCARV(C33;J33:K40;2;1);BUSCARV(C33;$M$31:$N$37;2;1))</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>=SI.ERROR(BUSCARV(C33;$J$31:$K$38;2;1);BUSCARV(C33;$M$31:$N$37;2;1))</v>
       </c>
       <c r="G33" s="12"/>
       <c r="H33" s="12"/>
-      <c r="J33" s="40">
+      <c r="J33" s="37">
         <v>5000</v>
       </c>
-      <c r="K33" s="39">
+      <c r="K33" s="36">
         <v>3.2500000000000001E-2</v>
       </c>
-      <c r="M33" s="40">
+      <c r="M33" s="37">
         <v>50000</v>
       </c>
-      <c r="N33" s="39">
+      <c r="N33" s="36">
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B34" s="4">
         <v>2</v>
       </c>
-      <c r="C34" s="40">
+      <c r="C34" s="37">
         <v>87401</v>
       </c>
-      <c r="D34" s="43">
-        <f t="shared" si="3"/>
+      <c r="D34" s="40">
+        <f t="shared" si="2"/>
         <v>0.08</v>
       </c>
       <c r="E34" s="4">
@@ -8790,36 +9056,36 @@
         <v>6992.08</v>
       </c>
       <c r="F34" s="12" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>=SI.ERROR(BUSCARV(C34;J34:K41;2;1);BUSCARV(C34;$M$31:$N$37;2;1))</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>=SI.ERROR(BUSCARV(C34;$J$31:$K$38;2;1);BUSCARV(C34;$M$31:$N$37;2;1))</v>
       </c>
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
-      <c r="J34" s="40">
+      <c r="J34" s="37">
         <v>10000</v>
       </c>
-      <c r="K34" s="39">
+      <c r="K34" s="36">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="M34" s="40">
+      <c r="M34" s="37">
         <v>100000</v>
       </c>
-      <c r="N34" s="39">
+      <c r="N34" s="36">
         <v>7.2499999999999995E-2</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B35" s="4">
         <v>6</v>
       </c>
-      <c r="C35" s="40">
+      <c r="C35" s="37">
         <v>310983</v>
       </c>
-      <c r="D35" s="43">
-        <f t="shared" si="3"/>
+      <c r="D35" s="40">
+        <f t="shared" si="2"/>
         <v>0.08</v>
       </c>
       <c r="E35" s="4">
@@ -8827,36 +9093,36 @@
         <v>24878.639999999999</v>
       </c>
       <c r="F35" s="12" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>=SI.ERROR(BUSCARV(C35;J35:K42;2;1);BUSCARV(C35;$M$31:$N$37;2;1))</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>=SI.ERROR(BUSCARV(C35;$J$31:$K$38;2;1);BUSCARV(C35;$M$31:$N$37;2;1))</v>
       </c>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
-      <c r="J35" s="40">
+      <c r="J35" s="37">
         <v>20000</v>
       </c>
-      <c r="K35" s="39">
+      <c r="K35" s="36">
         <v>0.05</v>
       </c>
-      <c r="M35" s="40">
+      <c r="M35" s="37">
         <v>200000</v>
       </c>
-      <c r="N35" s="39">
+      <c r="N35" s="36">
         <v>8.2500000000000004E-2</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B36" s="4">
         <v>3</v>
       </c>
-      <c r="C36" s="40">
+      <c r="C36" s="37">
         <v>43902</v>
       </c>
-      <c r="D36" s="43">
-        <f t="shared" si="3"/>
+      <c r="D36" s="40">
+        <f t="shared" si="2"/>
         <v>0.08</v>
       </c>
       <c r="E36" s="4">
@@ -8864,36 +9130,36 @@
         <v>3512.16</v>
       </c>
       <c r="F36" s="12" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>=SI.ERROR(BUSCARV(C36;J36:K43;2;1);BUSCARV(C36;$M$31:$N$37;2;1))</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>=SI.ERROR(BUSCARV(C36;$J$31:$K$38;2;1);BUSCARV(C36;$M$31:$N$37;2;1))</v>
       </c>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
-      <c r="J36" s="40">
+      <c r="J36" s="37">
         <v>25000</v>
       </c>
-      <c r="K36" s="39">
+      <c r="K36" s="36">
         <v>0.06</v>
       </c>
-      <c r="M36" s="40">
+      <c r="M36" s="37">
         <v>300000</v>
       </c>
-      <c r="N36" s="39">
+      <c r="N36" s="36">
         <v>9.2499999999999999E-2</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B37" s="4">
         <v>2</v>
       </c>
-      <c r="C37" s="40">
+      <c r="C37" s="37">
         <v>121021</v>
       </c>
-      <c r="D37" s="43">
-        <f t="shared" si="3"/>
+      <c r="D37" s="40">
+        <f t="shared" si="2"/>
         <v>0.08</v>
       </c>
       <c r="E37" s="4">
@@ -8901,36 +9167,36 @@
         <v>9681.68</v>
       </c>
       <c r="F37" s="12" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>=SI.ERROR(BUSCARV(C37;J37:K44;2;1);BUSCARV(C37;$M$31:$N$37;2;1))</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>=SI.ERROR(BUSCARV(C37;$J$31:$K$38;2;1);BUSCARV(C37;$M$31:$N$37;2;1))</v>
       </c>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
-      <c r="J37" s="40">
+      <c r="J37" s="37">
         <v>30000</v>
       </c>
-      <c r="K37" s="39">
+      <c r="K37" s="36">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M37" s="40">
+      <c r="M37" s="37">
         <v>500000</v>
       </c>
-      <c r="N37" s="39">
+      <c r="N37" s="36">
         <v>0.1</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B38" s="4">
         <v>3</v>
       </c>
-      <c r="C38" s="40">
+      <c r="C38" s="37">
         <v>908</v>
       </c>
-      <c r="D38" s="43">
-        <f t="shared" si="3"/>
+      <c r="D38" s="40">
+        <f t="shared" si="2"/>
         <v>0.02</v>
       </c>
       <c r="E38" s="4">
@@ -8938,30 +9204,30 @@
         <v>18.16</v>
       </c>
       <c r="F38" s="12" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>=SI.ERROR(BUSCARV(C38;J38:K45;2;1);BUSCARV(C38;$M$31:$N$37;2;1))</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>=SI.ERROR(BUSCARV(C38;$J$31:$K$38;2;1);BUSCARV(C38;$M$31:$N$37;2;1))</v>
       </c>
       <c r="G38" s="12"/>
       <c r="H38" s="12"/>
-      <c r="J38" s="40">
+      <c r="J38" s="37">
         <v>35000</v>
       </c>
-      <c r="K38" s="39">
+      <c r="K38" s="36">
         <v>0.08</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B39" s="4">
         <v>1</v>
       </c>
-      <c r="C39" s="40">
+      <c r="C39" s="37">
         <v>0</v>
       </c>
-      <c r="D39" s="43">
-        <f t="shared" si="3"/>
+      <c r="D39" s="40">
+        <f t="shared" si="2"/>
         <v>0.02</v>
       </c>
       <c r="E39" s="4">
@@ -8969,98 +9235,98 @@
         <v>0</v>
       </c>
       <c r="F39" s="12" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>=SI.ERROR(BUSCARV(C39;J39:K46;2;1);BUSCARV(C39;$M$31:$N$37;2;1))</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>=SI.ERROR(BUSCARV(C39;$J$31:$K$38;2;1);BUSCARV(C39;$M$31:$N$37;2;1))</v>
       </c>
       <c r="G39" s="12"/>
       <c r="H39" s="12"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B40" s="4">
         <v>4</v>
       </c>
-      <c r="C40" s="40">
+      <c r="C40" s="37">
         <v>359832</v>
       </c>
-      <c r="D40" s="43">
-        <f t="shared" si="3"/>
-        <v>9.2499999999999999E-2</v>
+      <c r="D40" s="40">
+        <f t="shared" si="2"/>
+        <v>0.08</v>
       </c>
       <c r="E40" s="4">
         <f t="shared" si="4"/>
-        <v>33284.46</v>
+        <v>28786.560000000001</v>
       </c>
       <c r="F40" s="12" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>=SI.ERROR(BUSCARV(C40;J40:K47;2;1);BUSCARV(C40;$M$31:$N$37;2;1))</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>=SI.ERROR(BUSCARV(C40;$J$31:$K$38;2;1);BUSCARV(C40;$M$31:$N$37;2;1))</v>
       </c>
       <c r="G40" s="12"/>
       <c r="H40" s="12"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B41" s="4">
         <v>4</v>
       </c>
-      <c r="C41" s="40">
+      <c r="C41" s="37">
         <v>502983</v>
       </c>
-      <c r="D41" s="43">
-        <f t="shared" si="3"/>
-        <v>0.1</v>
+      <c r="D41" s="40">
+        <f t="shared" si="2"/>
+        <v>0.08</v>
       </c>
       <c r="E41" s="4">
         <f t="shared" si="4"/>
-        <v>50298.3</v>
+        <v>40238.639999999999</v>
       </c>
       <c r="F41" s="12" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>=SI.ERROR(BUSCARV(C41;J41:K48;2;1);BUSCARV(C41;$M$31:$N$37;2;1))</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>=SI.ERROR(BUSCARV(C41;$J$31:$K$38;2;1);BUSCARV(C41;$M$31:$N$37;2;1))</v>
       </c>
       <c r="G41" s="12"/>
       <c r="H41" s="12"/>
     </row>
     <row r="46" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A48" s="35" t="s">
+      <c r="A48" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C48" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="B48" s="35" t="s">
+      <c r="D48" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="C48" s="35" t="s">
+      <c r="E48" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="J48" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="D48" s="35" t="s">
+      <c r="K48" s="44"/>
+      <c r="M48" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="E48" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="J48" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="K48" s="38"/>
-      <c r="M48" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="N48" s="37"/>
+      <c r="N48" s="45"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B49" s="4">
         <v>2</v>
@@ -9068,26 +9334,26 @@
       <c r="C49" s="4">
         <v>120000</v>
       </c>
-      <c r="D49" s="44"/>
+      <c r="D49" s="41"/>
       <c r="E49" s="4">
         <v>8400</v>
       </c>
-      <c r="J49" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="K49" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="M49" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="N49" s="36" t="s">
-        <v>102</v>
+      <c r="J49" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="K49" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="M49" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="N49" s="35" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B50" s="4">
         <v>1</v>
@@ -9095,7 +9361,7 @@
       <c r="C50" s="4">
         <v>210921</v>
       </c>
-      <c r="D50" s="44"/>
+      <c r="D50" s="41"/>
       <c r="E50" s="4">
         <v>14764.470000000001</v>
       </c>
@@ -9114,7 +9380,7 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B51" s="4">
         <v>1</v>
@@ -9122,7 +9388,7 @@
       <c r="C51" s="4">
         <v>100000</v>
       </c>
-      <c r="D51" s="44"/>
+      <c r="D51" s="41"/>
       <c r="E51" s="4">
         <v>7000.0000000000009</v>
       </c>
@@ -9141,7 +9407,7 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B52" s="4">
         <v>2</v>
@@ -9149,7 +9415,7 @@
       <c r="C52" s="4">
         <v>87401</v>
       </c>
-      <c r="D52" s="44"/>
+      <c r="D52" s="41"/>
       <c r="E52" s="4">
         <v>5244.0599999999995</v>
       </c>
@@ -9168,7 +9434,7 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B53" s="4">
         <v>6</v>
@@ -9176,7 +9442,7 @@
       <c r="C53" s="4">
         <v>310983</v>
       </c>
-      <c r="D53" s="44"/>
+      <c r="D53" s="41"/>
       <c r="E53" s="4">
         <v>28765.927499999998</v>
       </c>
@@ -9195,7 +9461,7 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B54" s="4">
         <v>3</v>
@@ -9203,7 +9469,7 @@
       <c r="C54" s="4">
         <v>43902</v>
       </c>
-      <c r="D54" s="44"/>
+      <c r="D54" s="41"/>
       <c r="E54" s="4">
         <v>878.04</v>
       </c>
@@ -9222,7 +9488,7 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B55" s="4">
         <v>2</v>
@@ -9230,7 +9496,7 @@
       <c r="C55" s="4">
         <v>121021</v>
       </c>
-      <c r="D55" s="44"/>
+      <c r="D55" s="41"/>
       <c r="E55" s="4">
         <v>8471.4700000000012</v>
       </c>
@@ -9249,7 +9515,7 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B56" s="4">
         <v>3</v>
@@ -9257,7 +9523,7 @@
       <c r="C56" s="4">
         <v>908</v>
       </c>
-      <c r="D56" s="44"/>
+      <c r="D56" s="41"/>
       <c r="E56" s="4">
         <v>18.16</v>
       </c>
@@ -9270,7 +9536,7 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B57" s="4">
         <v>1</v>
@@ -9278,14 +9544,14 @@
       <c r="C57" s="4">
         <v>0</v>
       </c>
-      <c r="D57" s="44"/>
+      <c r="D57" s="41"/>
       <c r="E57" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B58" s="4">
         <v>4</v>
@@ -9293,14 +9559,14 @@
       <c r="C58" s="4">
         <v>359832</v>
       </c>
-      <c r="D58" s="44"/>
+      <c r="D58" s="41"/>
       <c r="E58" s="4">
         <v>33284.46</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B59" s="4">
         <v>4</v>
@@ -9308,7 +9574,7 @@
       <c r="C59" s="4">
         <v>502983</v>
       </c>
-      <c r="D59" s="44"/>
+      <c r="D59" s="41"/>
       <c r="E59" s="4">
         <v>50298.3</v>
       </c>
@@ -9328,53 +9594,53 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8BB1D6C-BEAB-4376-8D52-1EBE08720090}">
-  <dimension ref="A9:L50"/>
+  <dimension ref="A9:L65"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="9" spans="1:12" ht="21" x14ac:dyDescent="0.4">
       <c r="A9" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="E12" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="D12" s="46" t="s">
-        <v>129</v>
-      </c>
-      <c r="E12" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="J12" s="36" t="s">
+      <c r="J12" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="L12" s="36" t="s">
-        <v>130</v>
+      <c r="K12" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="L12" s="35" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B13" s="4">
         <v>2892</v>
@@ -9389,14 +9655,14 @@
         <v>9381</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="K13" s="44"/>
-      <c r="L13" s="44"/>
+        <v>129</v>
+      </c>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B14" s="4">
         <v>3380</v>
@@ -9411,14 +9677,14 @@
         <v>10706</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="K14" s="44"/>
-      <c r="L14" s="44"/>
+        <v>130</v>
+      </c>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B15" s="4">
         <v>3744</v>
@@ -9433,14 +9699,14 @@
         <v>12279</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
+        <v>131</v>
+      </c>
+      <c r="K15" s="41"/>
+      <c r="L15" s="41"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B16" s="4">
         <v>3221</v>
@@ -9455,14 +9721,14 @@
         <v>6767</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="K16" s="44"/>
-      <c r="L16" s="44"/>
+        <v>132</v>
+      </c>
+      <c r="K16" s="41"/>
+      <c r="L16" s="41"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B17" s="4">
         <v>4839</v>
@@ -9477,14 +9743,14 @@
         <v>8832</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="K17" s="44"/>
-      <c r="L17" s="44"/>
+        <v>133</v>
+      </c>
+      <c r="K17" s="41"/>
+      <c r="L17" s="41"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B18" s="4">
         <v>3767</v>
@@ -9499,14 +9765,14 @@
         <v>12737</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="K18" s="44"/>
-      <c r="L18" s="44"/>
+        <v>134</v>
+      </c>
+      <c r="K18" s="41"/>
+      <c r="L18" s="41"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B19" s="4">
         <v>5467</v>
@@ -9521,14 +9787,14 @@
         <v>12036</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="K19" s="44"/>
-      <c r="L19" s="44"/>
+        <v>135</v>
+      </c>
+      <c r="K19" s="41"/>
+      <c r="L19" s="41"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B20" s="4">
         <v>3154</v>
@@ -9543,14 +9809,14 @@
         <v>9656</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="K20" s="44"/>
-      <c r="L20" s="44"/>
+        <v>136</v>
+      </c>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B21" s="4">
         <v>1718</v>
@@ -9565,14 +9831,14 @@
         <v>5321</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="K21" s="44"/>
-      <c r="L21" s="44"/>
+        <v>137</v>
+      </c>
+      <c r="K21" s="41"/>
+      <c r="L21" s="41"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B22" s="4">
         <v>1548</v>
@@ -9587,14 +9853,14 @@
         <v>5199</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="K22" s="44"/>
-      <c r="L22" s="44"/>
+        <v>138</v>
+      </c>
+      <c r="K22" s="41"/>
+      <c r="L22" s="41"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B23" s="4">
         <v>5083</v>
@@ -9609,14 +9875,14 @@
         <v>12601</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="K23" s="44"/>
-      <c r="L23" s="44"/>
+        <v>139</v>
+      </c>
+      <c r="K23" s="41"/>
+      <c r="L23" s="41"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B24" s="4">
         <v>5753</v>
@@ -9631,14 +9897,14 @@
         <v>11605</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="K24" s="44"/>
-      <c r="L24" s="44"/>
+        <v>140</v>
+      </c>
+      <c r="K24" s="41"/>
+      <c r="L24" s="41"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B25" s="4">
         <v>44566</v>
@@ -9653,14 +9919,14 @@
         <v>117120</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="K25" s="44"/>
-      <c r="L25" s="44"/>
+        <v>141</v>
+      </c>
+      <c r="K25" s="41"/>
+      <c r="L25" s="41"/>
     </row>
     <row r="31" spans="1:12" ht="21" x14ac:dyDescent="0.4">
       <c r="A31" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="21" x14ac:dyDescent="0.4">
@@ -9671,155 +9937,362 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="E35" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D36" t="s">
         <v>151</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="E36" t="s">
         <v>152</v>
       </c>
-      <c r="D36" t="s">
+      <c r="F36" t="s">
         <v>153</v>
-      </c>
-      <c r="E36" t="s">
-        <v>154</v>
-      </c>
-      <c r="F36" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" s="41" t="e" cm="1">
+        <f t="array" ref="B37">INDEX($F$35:$F$46,MATCH(MAKE&amp;MODEL,MAKES&amp;MODELS,0))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D37" t="s">
+        <v>151</v>
+      </c>
+      <c r="E37" t="s">
         <v>156</v>
       </c>
-      <c r="B37" s="44"/>
-      <c r="D37" t="s">
-        <v>153</v>
-      </c>
-      <c r="E37" t="s">
-        <v>158</v>
-      </c>
       <c r="F37" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
+        <v>158</v>
+      </c>
+      <c r="E38" t="s">
+        <v>159</v>
+      </c>
+      <c r="F38" t="s">
         <v>160</v>
-      </c>
-      <c r="E38" t="s">
-        <v>161</v>
-      </c>
-      <c r="F38" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E39" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F39" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
+        <v>163</v>
+      </c>
+      <c r="E40" t="s">
+        <v>164</v>
+      </c>
+      <c r="F40" t="s">
         <v>165</v>
-      </c>
-      <c r="E40" t="s">
-        <v>166</v>
-      </c>
-      <c r="F40" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E41" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F41" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
+        <v>168</v>
+      </c>
+      <c r="E42" t="s">
+        <v>169</v>
+      </c>
+      <c r="F42" t="s">
         <v>170</v>
-      </c>
-      <c r="E42" t="s">
-        <v>171</v>
-      </c>
-      <c r="F42" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D43" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E43" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F43" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E44" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F44" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E45" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F45" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D46" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E46" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F46" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B53" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B54" t="s">
+        <v>152</v>
+      </c>
+      <c r="D54" t="s">
+        <v>146</v>
+      </c>
+      <c r="E54" t="s">
+        <v>147</v>
+      </c>
+      <c r="F54" t="s">
+        <v>148</v>
+      </c>
+      <c r="G54" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B55" t="str" cm="1">
+        <f t="array" ref="B55">INDEX(CODES,MATCH(B53&amp;B54,MAKES&amp;MODELS,0))</f>
+        <v>C-094</v>
+      </c>
+      <c r="D55" t="s">
+        <v>151</v>
+      </c>
+      <c r="E55" t="s">
+        <v>152</v>
+      </c>
+      <c r="F55" t="s">
+        <v>153</v>
+      </c>
+      <c r="G55" t="str">
+        <f>D55&amp;E55</f>
+        <v>ChevySuburban</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D56" t="s">
+        <v>151</v>
+      </c>
+      <c r="E56" t="s">
+        <v>156</v>
+      </c>
+      <c r="F56" t="s">
+        <v>157</v>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" ref="G56:G65" si="0">D56&amp;E56</f>
+        <v>ChevyTahoe</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B57" t="str">
+        <f>INDEX(CODES,MATCH(B53&amp;B54,$G$54:$G$65,0))</f>
+        <v>C-094</v>
+      </c>
+      <c r="D57" t="s">
+        <v>158</v>
+      </c>
+      <c r="E57" t="s">
+        <v>159</v>
+      </c>
+      <c r="F57" t="s">
+        <v>160</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="0"/>
+        <v>FordExplorer</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D58" t="s">
+        <v>158</v>
+      </c>
+      <c r="E58" t="s">
+        <v>161</v>
+      </c>
+      <c r="F58" t="s">
+        <v>162</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="0"/>
+        <v>FordEscape</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D59" t="s">
+        <v>163</v>
+      </c>
+      <c r="E59" t="s">
+        <v>164</v>
+      </c>
+      <c r="F59" t="s">
+        <v>165</v>
+      </c>
+      <c r="G59" t="str">
+        <f t="shared" si="0"/>
+        <v>HondaPilot</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D60" t="s">
+        <v>163</v>
+      </c>
+      <c r="E60" t="s">
+        <v>166</v>
+      </c>
+      <c r="F60" t="s">
+        <v>167</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="0"/>
+        <v>HondaCR-V</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D61" t="s">
+        <v>168</v>
+      </c>
+      <c r="E61" t="s">
+        <v>169</v>
+      </c>
+      <c r="F61" t="s">
+        <v>170</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="0"/>
+        <v>JeepCompass</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D62" t="s">
+        <v>168</v>
+      </c>
+      <c r="E62" t="s">
+        <v>171</v>
+      </c>
+      <c r="F62" t="s">
+        <v>172</v>
+      </c>
+      <c r="G62" t="str">
+        <f t="shared" si="0"/>
+        <v>JeepGrand Cherokee</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D63" t="s">
+        <v>173</v>
+      </c>
+      <c r="E63" t="s">
+        <v>152</v>
+      </c>
+      <c r="F63" t="s">
+        <v>174</v>
+      </c>
+      <c r="G63" t="str">
+        <f t="shared" si="0"/>
+        <v>NissanSuburban</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D64" t="s">
+        <v>145</v>
+      </c>
+      <c r="E64" t="s">
+        <v>150</v>
+      </c>
+      <c r="F64" t="s">
+        <v>155</v>
+      </c>
+      <c r="G64" t="str">
+        <f t="shared" si="0"/>
+        <v>ToyotaSequoia</v>
+      </c>
+    </row>
+    <row r="65" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D65" t="s">
+        <v>145</v>
+      </c>
+      <c r="E65" t="s">
+        <v>175</v>
+      </c>
+      <c r="F65" t="s">
+        <v>176</v>
+      </c>
+      <c r="G65" t="str">
+        <f t="shared" si="0"/>
+        <v>ToyotaLand Cruiser</v>
       </c>
     </row>
   </sheetData>

</xml_diff>